<commit_message>
Test Cases increased and Updated to 17
</commit_message>
<xml_diff>
--- a/documentation/1.0 Requirements/Traceability Matrix 1.0 OS Scheduler.xlsx
+++ b/documentation/1.0 Requirements/Traceability Matrix 1.0 OS Scheduler.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="95">
   <si>
     <t>Program</t>
   </si>
@@ -81,12 +81,6 @@
   </si>
   <si>
     <t>Reference Document</t>
-  </si>
-  <si>
-    <t>functional</t>
-  </si>
-  <si>
-    <t>File structure</t>
   </si>
   <si>
     <t>No functional</t>
@@ -109,9 +103,6 @@
     <t>Sergio,Esteban,Miguel</t>
   </si>
   <si>
-    <t>DSD 0.0 OS Scheduler.docx</t>
-  </si>
-  <si>
     <t>Scheduler Initialization</t>
   </si>
   <si>
@@ -161,12 +152,170 @@
   </si>
   <si>
     <t>OS Scheduler</t>
+  </si>
+  <si>
+    <t>The Scheduler module shall provide interface to support Initialization, De-Initialization, Start, Os-Tick, Back Ground Task &amp; Task Callback functions</t>
+  </si>
+  <si>
+    <t>Scheduler initialization shall be supported through SchM_Init API</t>
+  </si>
+  <si>
+    <t>Scheduler De-Initialization shall be supported through SchM_DeInit API</t>
+  </si>
+  <si>
+    <t>Scheduler Start shall be supported through SchM_Start API</t>
+  </si>
+  <si>
+    <t>1.8</t>
+  </si>
+  <si>
+    <t>Design concept</t>
+  </si>
+  <si>
+    <t>OS Tick Callback shall be supported through SchM_OsTick API</t>
+  </si>
+  <si>
+    <t>DSD 1.0 OS Scheduler.docx</t>
+  </si>
+  <si>
+    <t>Background task shall be supported through SchM_Background API</t>
+  </si>
+  <si>
+    <t>Callback functions shall be referred as per the task period: 
+SchM_Task_##period(void)
+E.g. SchM_Task_1p56ms(void)</t>
+  </si>
+  <si>
+    <t>WorkLoad_Scheduler.xlsx</t>
+  </si>
+  <si>
+    <t>Practice II - Scheduler.pdf</t>
+  </si>
+  <si>
+    <t>1.9</t>
+  </si>
+  <si>
+    <t>Portability</t>
+  </si>
+  <si>
+    <t>The Scheduler has to be designed in a manner that it can be portable between different platforms</t>
+  </si>
+  <si>
+    <t>1.10</t>
+  </si>
+  <si>
+    <t>Module Design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scheduler Module Shall be allocated at BSW and Services layer from AUTOSAR </t>
+  </si>
+  <si>
+    <t>The Design concept shall be based on the OS Tick, mask and offset concepts</t>
+  </si>
+  <si>
+    <t>Scheduler Design</t>
+  </si>
+  <si>
+    <t>1.11</t>
+  </si>
+  <si>
+    <t>File Structure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Files containing Configuration, Main functionality, type definitions &amp; tasks allocation shall be provided </t>
+  </si>
+  <si>
+    <t>SchM.c,SchM.h,SchM_cfg.h, SchM_cfg.c, SchM_Tasks.c, SchM_Tasks.h</t>
+  </si>
+  <si>
+    <t>1.12</t>
+  </si>
+  <si>
+    <t>Configuration Files</t>
+  </si>
+  <si>
+    <t>SchM_Cfg.c &amp; SchM_Cfg.h shall provide the task configuration table</t>
+  </si>
+  <si>
+    <t>SchM_Cfg.c, SchM_Cfg.h</t>
+  </si>
+  <si>
+    <t>1.13</t>
+  </si>
+  <si>
+    <t>Main functionality</t>
+  </si>
+  <si>
+    <t>SchM.c &amp; SchM.h shall provide the main functionality of the Scheduler. OS-Tick callback shall be allocated in these files</t>
+  </si>
+  <si>
+    <t>SchM_Types.h</t>
+  </si>
+  <si>
+    <t>1.14</t>
+  </si>
+  <si>
+    <t>Type definitions</t>
+  </si>
+  <si>
+    <t>SchM_Types.h shall provide the Scheduler type definitions</t>
+  </si>
+  <si>
+    <t>1.16</t>
+  </si>
+  <si>
+    <t>Tasks allocation</t>
+  </si>
+  <si>
+    <t>SchM_Tasks.c &amp; SchM_Tasks.h shall allocate the module's periodic tasks</t>
+  </si>
+  <si>
+    <t>OS Scheduler Project</t>
+  </si>
+  <si>
+    <t>1.17</t>
+  </si>
+  <si>
+    <t>Test_Software_Spec.docx</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Functional</t>
+  </si>
+  <si>
+    <t>Task Excercise</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>1.15</t>
+  </si>
+  <si>
+    <t>Turn a Pin level ON at the entrance of a task and turn the Pin level OFF at the end of a task excecution</t>
+  </si>
+  <si>
+    <t>CPU Load</t>
+  </si>
+  <si>
+    <t>Turn a pin level ON before entering the Background Task and turn the pin level OFF at the end of the Background Task</t>
+  </si>
+  <si>
+    <t>Modify CPU Load</t>
+  </si>
+  <si>
+    <t>Modify the CPU Load by adding workload to the tasks</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="9">
     <font>
       <sz val="10"/>
@@ -219,10 +368,9 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="12"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -433,7 +581,7 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -507,9 +655,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -519,9 +664,19 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -555,6 +710,21 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -577,13 +747,14 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="164" formatCode="0.0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1117,8 +1288,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A7:L50" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A7:L50"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A7:L49" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A7:L49"/>
   <tableColumns count="12">
     <tableColumn id="1" name=" " dataDxfId="11"/>
     <tableColumn id="2" name="Req. ID" dataDxfId="10"/>
@@ -1130,8 +1301,8 @@
     <tableColumn id="8" name="Comments2" dataDxfId="4"/>
     <tableColumn id="9" name="File Reference" dataDxfId="3"/>
     <tableColumn id="11" name="Comments3" dataDxfId="2"/>
-    <tableColumn id="12" name="Test Case Reference" dataDxfId="1"/>
-    <tableColumn id="13" name="Result" dataDxfId="0"/>
+    <tableColumn id="12" name="Test Case Reference" dataDxfId="0"/>
+    <tableColumn id="13" name="Result" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1425,11 +1596,11 @@
   <sheetPr codeName="Sheet3">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IF65362"/>
+  <dimension ref="A1:IF65361"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomLeft" activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" outlineLevelCol="1"/>
@@ -1442,9 +1613,9 @@
     <col min="6" max="6" width="62.28515625" style="10" customWidth="1" outlineLevel="1"/>
     <col min="7" max="7" width="32.7109375" style="11" bestFit="1" customWidth="1" outlineLevel="1"/>
     <col min="8" max="8" width="21.28515625" style="11" bestFit="1" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="24.140625" style="11" bestFit="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="9" max="9" width="33" style="11" bestFit="1" customWidth="1" outlineLevel="1" collapsed="1"/>
     <col min="10" max="10" width="21.28515625" style="11" bestFit="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="11" max="11" width="32.28515625" style="8" bestFit="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="11" max="11" width="32.28515625" style="53" bestFit="1" customWidth="1" outlineLevel="1" collapsed="1"/>
     <col min="12" max="12" width="19" style="8" customWidth="1" outlineLevel="1"/>
     <col min="13" max="16384" width="9.140625" style="8"/>
   </cols>
@@ -1459,46 +1630,46 @@
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
+      <c r="K1" s="48"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" ht="21.6" customHeight="1" thickTop="1">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="35"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="38"/>
       <c r="D2" s="18" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1">
-      <c r="A3" s="36"/>
-      <c r="B3" s="36"/>
-      <c r="C3" s="37"/>
+      <c r="A3" s="39"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="40"/>
       <c r="D3" s="18" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
+      <c r="K3" s="48"/>
     </row>
     <row r="4" spans="1:12" s="1" customFormat="1">
-      <c r="A4" s="36"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="40"/>
       <c r="D4" s="18" t="s">
         <v>20</v>
       </c>
@@ -1508,50 +1679,50 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
+      <c r="K4" s="48"/>
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" ht="45">
-      <c r="A5" s="36"/>
-      <c r="B5" s="36"/>
-      <c r="C5" s="37"/>
+      <c r="A5" s="39"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="40"/>
       <c r="D5" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="30" t="s">
-        <v>25</v>
+      <c r="E5" s="29" t="s">
+        <v>23</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="K5" s="48"/>
     </row>
     <row r="6" spans="1:12" s="1" customFormat="1" ht="45.75" thickBot="1">
-      <c r="A6" s="38"/>
-      <c r="B6" s="38"/>
-      <c r="C6" s="39"/>
+      <c r="A6" s="41"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="42"/>
       <c r="D6" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="30" t="s">
-        <v>25</v>
+      <c r="E6" s="29" t="s">
+        <v>23</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="40" t="s">
+      <c r="G6" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="42"/>
-      <c r="I6" s="43" t="s">
+      <c r="H6" s="45"/>
+      <c r="I6" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="J6" s="44"/>
-      <c r="K6" s="40" t="s">
+      <c r="J6" s="47"/>
+      <c r="K6" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="L6" s="41"/>
+      <c r="L6" s="44"/>
     </row>
     <row r="7" spans="1:12" s="6" customFormat="1" ht="16.5" thickTop="1">
       <c r="A7" s="16" t="s">
@@ -1567,7 +1738,7 @@
         <v>3</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>4</v>
@@ -1584,348 +1755,560 @@
       <c r="J7" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="K7" s="6" t="s">
+      <c r="K7" s="49" t="s">
         <v>18</v>
       </c>
       <c r="L7" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="4" customFormat="1">
+    <row r="8" spans="1:12" s="4" customFormat="1" ht="45.75">
       <c r="A8" s="12"/>
       <c r="B8" s="19" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="29"/>
+        <v>26</v>
+      </c>
+      <c r="F8" s="32" t="s">
+        <v>44</v>
+      </c>
       <c r="G8" s="15"/>
       <c r="H8" s="15"/>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
-      <c r="K8" s="14" t="s">
-        <v>24</v>
+      <c r="K8" s="50" t="s">
+        <v>22</v>
       </c>
       <c r="L8" s="14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="4" customFormat="1" ht="31.5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="4" customFormat="1" ht="35.25" customHeight="1">
       <c r="A9" s="12"/>
       <c r="B9" s="19" t="s">
-        <v>37</v>
+        <v>88</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>21</v>
+        <v>86</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="14"/>
+        <v>26</v>
+      </c>
+      <c r="F9" s="34" t="s">
+        <v>45</v>
+      </c>
       <c r="G9" s="15" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="H9" s="15"/>
-      <c r="I9" s="32" t="s">
-        <v>45</v>
+      <c r="I9" s="31" t="s">
+        <v>40</v>
       </c>
       <c r="J9" s="15"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="31"/>
-    </row>
-    <row r="10" spans="1:12" s="4" customFormat="1" ht="31.5">
+      <c r="K9" s="50">
+        <v>1</v>
+      </c>
+      <c r="L9" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="4" customFormat="1" ht="35.25" customHeight="1">
       <c r="A10" s="12"/>
       <c r="B10" s="19" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>21</v>
+        <v>86</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" s="14"/>
+        <v>26</v>
+      </c>
+      <c r="F10" s="34" t="s">
+        <v>46</v>
+      </c>
       <c r="G10" s="15" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="H10" s="15"/>
-      <c r="I10" s="32" t="s">
-        <v>45</v>
+      <c r="I10" s="31" t="s">
+        <v>42</v>
       </c>
       <c r="J10" s="15"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="31"/>
+      <c r="K10" s="50">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="L10" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="11" spans="1:12" s="4" customFormat="1">
       <c r="A11" s="12"/>
       <c r="B11" s="19" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>21</v>
+        <v>86</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="14"/>
+        <v>26</v>
+      </c>
+      <c r="F11" s="35" t="s">
+        <v>47</v>
+      </c>
       <c r="G11" s="15" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="H11" s="15"/>
-      <c r="I11" s="32" t="s">
-        <v>43</v>
+      <c r="I11" s="31" t="s">
+        <v>40</v>
       </c>
       <c r="J11" s="15"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="31"/>
+      <c r="K11" s="50">
+        <v>1.2</v>
+      </c>
+      <c r="L11" s="30" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="12" spans="1:12" s="4" customFormat="1">
       <c r="A12" s="12"/>
       <c r="B12" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12" s="15"/>
+      <c r="I12" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="14"/>
-      <c r="G12" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="H12" s="15"/>
-      <c r="I12" s="32" t="s">
-        <v>43</v>
-      </c>
       <c r="J12" s="15"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="31"/>
-    </row>
-    <row r="13" spans="1:12" s="4" customFormat="1">
+      <c r="K12" s="50">
+        <v>1.3</v>
+      </c>
+      <c r="L12" s="30" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="4" customFormat="1" ht="30">
       <c r="A13" s="12"/>
       <c r="B13" s="19" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>21</v>
+        <v>86</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="14"/>
+        <v>31</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="34" t="s">
+        <v>52</v>
+      </c>
       <c r="G13" s="15" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="H13" s="15"/>
-      <c r="I13" s="32" t="s">
-        <v>43</v>
+      <c r="I13" s="31" t="s">
+        <v>40</v>
       </c>
       <c r="J13" s="15"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="31"/>
-    </row>
-    <row r="14" spans="1:12" s="4" customFormat="1" ht="31.5">
+      <c r="K13" s="50">
+        <v>1.4</v>
+      </c>
+      <c r="L13" s="30" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="4" customFormat="1" ht="45.75">
       <c r="A14" s="12"/>
       <c r="B14" s="19" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>21</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="14"/>
+        <v>26</v>
+      </c>
+      <c r="F14" s="33" t="s">
+        <v>53</v>
+      </c>
       <c r="G14" s="15" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="H14" s="15"/>
-      <c r="I14" s="32" t="s">
-        <v>44</v>
+      <c r="I14" s="31" t="s">
+        <v>41</v>
       </c>
       <c r="J14" s="15"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="31"/>
-    </row>
-    <row r="15" spans="1:12" s="4" customFormat="1">
+      <c r="K14" s="50">
+        <v>1.5</v>
+      </c>
+      <c r="L14" s="30" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="4" customFormat="1" ht="30">
       <c r="A15" s="12"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="15"/>
+      <c r="B15" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="G15" s="36" t="s">
+        <v>55</v>
+      </c>
       <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
+      <c r="I15" s="15" t="s">
+        <v>54</v>
+      </c>
       <c r="J15" s="15"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-    </row>
-    <row r="16" spans="1:12" s="4" customFormat="1">
+      <c r="K15" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="L15" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="4" customFormat="1" ht="30">
       <c r="A16" s="12"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
+      <c r="B16" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="34" t="s">
+        <v>58</v>
+      </c>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
+      <c r="I16" s="15" t="s">
+        <v>82</v>
+      </c>
       <c r="J16" s="15"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-    </row>
-    <row r="17" spans="1:12" s="4" customFormat="1">
+      <c r="K16" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="L16" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" s="4" customFormat="1" ht="30.75">
       <c r="A17" s="12"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
+      <c r="B17" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="33" t="s">
+        <v>61</v>
+      </c>
       <c r="G17" s="15"/>
       <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
+      <c r="I17" s="15" t="s">
+        <v>82</v>
+      </c>
       <c r="J17" s="15"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-    </row>
-    <row r="18" spans="1:12" s="4" customFormat="1">
+      <c r="K17" s="50">
+        <v>1.6</v>
+      </c>
+      <c r="L17" s="30" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" s="4" customFormat="1" ht="47.25">
       <c r="A18" s="12"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
+      <c r="B18" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="34" t="s">
+        <v>66</v>
+      </c>
       <c r="G18" s="15"/>
       <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
+      <c r="I18" s="31" t="s">
+        <v>67</v>
+      </c>
       <c r="J18" s="15"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
-    </row>
-    <row r="19" spans="1:12" s="4" customFormat="1">
+      <c r="K18" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="L18" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" s="4" customFormat="1" ht="30">
       <c r="A19" s="12"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
+      <c r="B19" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" s="34" t="s">
+        <v>70</v>
+      </c>
       <c r="G19" s="15"/>
       <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
+      <c r="I19" s="15" t="s">
+        <v>71</v>
+      </c>
       <c r="J19" s="15"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="12"/>
-    </row>
-    <row r="20" spans="1:12" s="4" customFormat="1">
+      <c r="K19" s="50">
+        <v>1.7</v>
+      </c>
+      <c r="L19" s="30" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" s="4" customFormat="1" ht="30">
       <c r="A20" s="12"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
+      <c r="B20" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" s="34" t="s">
+        <v>74</v>
+      </c>
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
+      <c r="I20" s="31" t="s">
+        <v>40</v>
+      </c>
       <c r="J20" s="15"/>
-      <c r="K20" s="12"/>
-      <c r="L20" s="12"/>
+      <c r="K20" s="50">
+        <v>1.8</v>
+      </c>
+      <c r="L20" s="30" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="21" spans="1:12" s="4" customFormat="1">
       <c r="A21" s="12"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
+      <c r="B21" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" s="35" t="s">
+        <v>78</v>
+      </c>
       <c r="G21" s="15"/>
       <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
+      <c r="I21" s="15" t="s">
+        <v>75</v>
+      </c>
       <c r="J21" s="15"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="12"/>
-    </row>
-    <row r="22" spans="1:12" s="4" customFormat="1">
+      <c r="K21" s="50">
+        <v>1.9</v>
+      </c>
+      <c r="L21" s="30" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" s="4" customFormat="1" ht="31.5">
       <c r="A22" s="12"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
+      <c r="B22" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" s="34" t="s">
+        <v>81</v>
+      </c>
       <c r="G22" s="15"/>
       <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
+      <c r="I22" s="31" t="s">
+        <v>41</v>
+      </c>
       <c r="J22" s="15"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="12"/>
-    </row>
-    <row r="23" spans="1:12" s="4" customFormat="1">
+      <c r="K22" s="54">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="L22" s="30" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" s="4" customFormat="1" ht="30">
       <c r="A23" s="12"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
+      <c r="B23" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D23" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" s="34" t="s">
+        <v>90</v>
+      </c>
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
+      <c r="I23" s="15" t="s">
+        <v>84</v>
+      </c>
       <c r="J23" s="15"/>
-      <c r="K23" s="12"/>
-      <c r="L23" s="12"/>
-    </row>
-    <row r="24" spans="1:12" s="4" customFormat="1">
+      <c r="K23" s="54">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="L23" s="30" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A24" s="12"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
+      <c r="B24" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="34" t="s">
+        <v>92</v>
+      </c>
       <c r="G24" s="15"/>
       <c r="H24" s="15"/>
       <c r="I24" s="15"/>
       <c r="J24" s="15"/>
-      <c r="K24" s="12"/>
-      <c r="L24" s="12"/>
+      <c r="K24" s="54">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="L24" s="30" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="25" spans="1:12" s="4" customFormat="1">
       <c r="A25" s="12"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
+      <c r="B25" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" s="34" t="s">
+        <v>94</v>
+      </c>
       <c r="G25" s="15"/>
       <c r="H25" s="15"/>
       <c r="I25" s="15"/>
       <c r="J25" s="15"/>
-      <c r="K25" s="12"/>
-      <c r="L25" s="12"/>
+      <c r="K25" s="54">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="L25" s="30" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="26" spans="1:12" s="4" customFormat="1">
       <c r="A26" s="12"/>
@@ -1938,7 +2321,7 @@
       <c r="H26" s="15"/>
       <c r="I26" s="15"/>
       <c r="J26" s="15"/>
-      <c r="K26" s="12"/>
+      <c r="K26" s="51"/>
       <c r="L26" s="12"/>
     </row>
     <row r="27" spans="1:12" s="4" customFormat="1">
@@ -1952,7 +2335,7 @@
       <c r="H27" s="15"/>
       <c r="I27" s="15"/>
       <c r="J27" s="15"/>
-      <c r="K27" s="12"/>
+      <c r="K27" s="51"/>
       <c r="L27" s="12"/>
     </row>
     <row r="28" spans="1:12" s="4" customFormat="1">
@@ -1966,7 +2349,7 @@
       <c r="H28" s="15"/>
       <c r="I28" s="15"/>
       <c r="J28" s="15"/>
-      <c r="K28" s="12"/>
+      <c r="K28" s="51"/>
       <c r="L28" s="12"/>
     </row>
     <row r="29" spans="1:12" s="4" customFormat="1">
@@ -1980,7 +2363,7 @@
       <c r="H29" s="15"/>
       <c r="I29" s="15"/>
       <c r="J29" s="15"/>
-      <c r="K29" s="12"/>
+      <c r="K29" s="51"/>
       <c r="L29" s="12"/>
     </row>
     <row r="30" spans="1:12" s="4" customFormat="1">
@@ -1994,7 +2377,7 @@
       <c r="H30" s="15"/>
       <c r="I30" s="15"/>
       <c r="J30" s="15"/>
-      <c r="K30" s="12"/>
+      <c r="K30" s="51"/>
       <c r="L30" s="12"/>
     </row>
     <row r="31" spans="1:12" s="4" customFormat="1">
@@ -2008,7 +2391,7 @@
       <c r="H31" s="15"/>
       <c r="I31" s="15"/>
       <c r="J31" s="15"/>
-      <c r="K31" s="12"/>
+      <c r="K31" s="51"/>
       <c r="L31" s="12"/>
     </row>
     <row r="32" spans="1:12" s="4" customFormat="1">
@@ -2022,7 +2405,7 @@
       <c r="H32" s="15"/>
       <c r="I32" s="15"/>
       <c r="J32" s="15"/>
-      <c r="K32" s="12"/>
+      <c r="K32" s="51"/>
       <c r="L32" s="12"/>
     </row>
     <row r="33" spans="1:12" s="4" customFormat="1">
@@ -2036,7 +2419,7 @@
       <c r="H33" s="15"/>
       <c r="I33" s="15"/>
       <c r="J33" s="15"/>
-      <c r="K33" s="12"/>
+      <c r="K33" s="51"/>
       <c r="L33" s="12"/>
     </row>
     <row r="34" spans="1:12" s="4" customFormat="1">
@@ -2050,7 +2433,7 @@
       <c r="H34" s="15"/>
       <c r="I34" s="15"/>
       <c r="J34" s="15"/>
-      <c r="K34" s="12"/>
+      <c r="K34" s="51"/>
       <c r="L34" s="12"/>
     </row>
     <row r="35" spans="1:12" s="4" customFormat="1">
@@ -2064,7 +2447,7 @@
       <c r="H35" s="15"/>
       <c r="I35" s="15"/>
       <c r="J35" s="15"/>
-      <c r="K35" s="12"/>
+      <c r="K35" s="51"/>
       <c r="L35" s="12"/>
     </row>
     <row r="36" spans="1:12" s="4" customFormat="1">
@@ -2078,7 +2461,7 @@
       <c r="H36" s="15"/>
       <c r="I36" s="15"/>
       <c r="J36" s="15"/>
-      <c r="K36" s="12"/>
+      <c r="K36" s="51"/>
       <c r="L36" s="12"/>
     </row>
     <row r="37" spans="1:12" s="4" customFormat="1">
@@ -2092,7 +2475,7 @@
       <c r="H37" s="15"/>
       <c r="I37" s="15"/>
       <c r="J37" s="15"/>
-      <c r="K37" s="12"/>
+      <c r="K37" s="51"/>
       <c r="L37" s="12"/>
     </row>
     <row r="38" spans="1:12" s="4" customFormat="1">
@@ -2106,7 +2489,7 @@
       <c r="H38" s="15"/>
       <c r="I38" s="15"/>
       <c r="J38" s="15"/>
-      <c r="K38" s="12"/>
+      <c r="K38" s="51"/>
       <c r="L38" s="12"/>
     </row>
     <row r="39" spans="1:12" s="4" customFormat="1">
@@ -2120,7 +2503,7 @@
       <c r="H39" s="15"/>
       <c r="I39" s="15"/>
       <c r="J39" s="15"/>
-      <c r="K39" s="12"/>
+      <c r="K39" s="51"/>
       <c r="L39" s="12"/>
     </row>
     <row r="40" spans="1:12" s="4" customFormat="1">
@@ -2134,7 +2517,7 @@
       <c r="H40" s="15"/>
       <c r="I40" s="15"/>
       <c r="J40" s="15"/>
-      <c r="K40" s="12"/>
+      <c r="K40" s="51"/>
       <c r="L40" s="12"/>
     </row>
     <row r="41" spans="1:12" s="4" customFormat="1">
@@ -2148,7 +2531,7 @@
       <c r="H41" s="15"/>
       <c r="I41" s="15"/>
       <c r="J41" s="15"/>
-      <c r="K41" s="12"/>
+      <c r="K41" s="51"/>
       <c r="L41" s="12"/>
     </row>
     <row r="42" spans="1:12" s="4" customFormat="1">
@@ -2162,7 +2545,7 @@
       <c r="H42" s="15"/>
       <c r="I42" s="15"/>
       <c r="J42" s="15"/>
-      <c r="K42" s="12"/>
+      <c r="K42" s="51"/>
       <c r="L42" s="12"/>
     </row>
     <row r="43" spans="1:12" s="4" customFormat="1">
@@ -2176,7 +2559,7 @@
       <c r="H43" s="15"/>
       <c r="I43" s="15"/>
       <c r="J43" s="15"/>
-      <c r="K43" s="12"/>
+      <c r="K43" s="51"/>
       <c r="L43" s="12"/>
     </row>
     <row r="44" spans="1:12" s="4" customFormat="1">
@@ -2190,7 +2573,7 @@
       <c r="H44" s="15"/>
       <c r="I44" s="15"/>
       <c r="J44" s="15"/>
-      <c r="K44" s="12"/>
+      <c r="K44" s="51"/>
       <c r="L44" s="12"/>
     </row>
     <row r="45" spans="1:12" s="4" customFormat="1">
@@ -2204,7 +2587,7 @@
       <c r="H45" s="15"/>
       <c r="I45" s="15"/>
       <c r="J45" s="15"/>
-      <c r="K45" s="12"/>
+      <c r="K45" s="51"/>
       <c r="L45" s="12"/>
     </row>
     <row r="46" spans="1:12" s="4" customFormat="1">
@@ -2218,7 +2601,7 @@
       <c r="H46" s="15"/>
       <c r="I46" s="15"/>
       <c r="J46" s="15"/>
-      <c r="K46" s="12"/>
+      <c r="K46" s="51"/>
       <c r="L46" s="12"/>
     </row>
     <row r="47" spans="1:12" s="4" customFormat="1">
@@ -2232,7 +2615,7 @@
       <c r="H47" s="15"/>
       <c r="I47" s="15"/>
       <c r="J47" s="15"/>
-      <c r="K47" s="12"/>
+      <c r="K47" s="51"/>
       <c r="L47" s="12"/>
     </row>
     <row r="48" spans="1:12" s="4" customFormat="1">
@@ -2246,7 +2629,7 @@
       <c r="H48" s="15"/>
       <c r="I48" s="15"/>
       <c r="J48" s="15"/>
-      <c r="K48" s="12"/>
+      <c r="K48" s="51"/>
       <c r="L48" s="12"/>
     </row>
     <row r="49" spans="1:12" s="4" customFormat="1">
@@ -2260,22 +2643,20 @@
       <c r="H49" s="15"/>
       <c r="I49" s="15"/>
       <c r="J49" s="15"/>
-      <c r="K49" s="12"/>
+      <c r="K49" s="51"/>
       <c r="L49" s="12"/>
     </row>
     <row r="50" spans="1:12" s="4" customFormat="1">
-      <c r="A50" s="12"/>
-      <c r="B50" s="19"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="26"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="15"/>
-      <c r="H50" s="15"/>
-      <c r="I50" s="15"/>
-      <c r="J50" s="15"/>
-      <c r="K50" s="12"/>
-      <c r="L50" s="12"/>
+      <c r="B50" s="22"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="27"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="7"/>
+      <c r="I50" s="7"/>
+      <c r="J50" s="7"/>
+      <c r="K50" s="52"/>
     </row>
     <row r="51" spans="1:12" s="4" customFormat="1">
       <c r="B51" s="22"/>
@@ -2287,6 +2668,7 @@
       <c r="H51" s="7"/>
       <c r="I51" s="7"/>
       <c r="J51" s="7"/>
+      <c r="K51" s="52"/>
     </row>
     <row r="52" spans="1:12" s="4" customFormat="1">
       <c r="B52" s="22"/>
@@ -2298,6 +2680,7 @@
       <c r="H52" s="7"/>
       <c r="I52" s="7"/>
       <c r="J52" s="7"/>
+      <c r="K52" s="52"/>
     </row>
     <row r="53" spans="1:12" s="4" customFormat="1">
       <c r="B53" s="22"/>
@@ -2309,6 +2692,7 @@
       <c r="H53" s="7"/>
       <c r="I53" s="7"/>
       <c r="J53" s="7"/>
+      <c r="K53" s="52"/>
     </row>
     <row r="54" spans="1:12" s="4" customFormat="1">
       <c r="B54" s="22"/>
@@ -2320,6 +2704,7 @@
       <c r="H54" s="7"/>
       <c r="I54" s="7"/>
       <c r="J54" s="7"/>
+      <c r="K54" s="52"/>
     </row>
     <row r="55" spans="1:12" s="4" customFormat="1">
       <c r="B55" s="22"/>
@@ -2331,6 +2716,7 @@
       <c r="H55" s="7"/>
       <c r="I55" s="7"/>
       <c r="J55" s="7"/>
+      <c r="K55" s="52"/>
     </row>
     <row r="56" spans="1:12" s="4" customFormat="1">
       <c r="B56" s="22"/>
@@ -2342,6 +2728,7 @@
       <c r="H56" s="7"/>
       <c r="I56" s="7"/>
       <c r="J56" s="7"/>
+      <c r="K56" s="52"/>
     </row>
     <row r="57" spans="1:12" s="4" customFormat="1">
       <c r="B57" s="22"/>
@@ -2353,6 +2740,7 @@
       <c r="H57" s="7"/>
       <c r="I57" s="7"/>
       <c r="J57" s="7"/>
+      <c r="K57" s="52"/>
     </row>
     <row r="58" spans="1:12" s="4" customFormat="1">
       <c r="B58" s="22"/>
@@ -2364,6 +2752,7 @@
       <c r="H58" s="7"/>
       <c r="I58" s="7"/>
       <c r="J58" s="7"/>
+      <c r="K58" s="52"/>
     </row>
     <row r="59" spans="1:12" s="4" customFormat="1">
       <c r="B59" s="22"/>
@@ -2375,6 +2764,7 @@
       <c r="H59" s="7"/>
       <c r="I59" s="7"/>
       <c r="J59" s="7"/>
+      <c r="K59" s="52"/>
     </row>
     <row r="60" spans="1:12" s="4" customFormat="1">
       <c r="B60" s="22"/>
@@ -2386,6 +2776,7 @@
       <c r="H60" s="7"/>
       <c r="I60" s="7"/>
       <c r="J60" s="7"/>
+      <c r="K60" s="52"/>
     </row>
     <row r="61" spans="1:12" s="4" customFormat="1">
       <c r="B61" s="22"/>
@@ -2397,6 +2788,7 @@
       <c r="H61" s="7"/>
       <c r="I61" s="7"/>
       <c r="J61" s="7"/>
+      <c r="K61" s="52"/>
     </row>
     <row r="62" spans="1:12" s="4" customFormat="1">
       <c r="B62" s="22"/>
@@ -2408,6 +2800,7 @@
       <c r="H62" s="7"/>
       <c r="I62" s="7"/>
       <c r="J62" s="7"/>
+      <c r="K62" s="52"/>
     </row>
     <row r="63" spans="1:12" s="4" customFormat="1">
       <c r="B63" s="22"/>
@@ -2419,6 +2812,7 @@
       <c r="H63" s="7"/>
       <c r="I63" s="7"/>
       <c r="J63" s="7"/>
+      <c r="K63" s="52"/>
     </row>
     <row r="64" spans="1:12" s="4" customFormat="1">
       <c r="B64" s="22"/>
@@ -2430,8 +2824,9 @@
       <c r="H64" s="7"/>
       <c r="I64" s="7"/>
       <c r="J64" s="7"/>
-    </row>
-    <row r="65" spans="2:10" s="4" customFormat="1">
+      <c r="K64" s="52"/>
+    </row>
+    <row r="65" spans="2:11" s="4" customFormat="1">
       <c r="B65" s="22"/>
       <c r="C65" s="5"/>
       <c r="D65" s="27"/>
@@ -2441,8 +2836,9 @@
       <c r="H65" s="7"/>
       <c r="I65" s="7"/>
       <c r="J65" s="7"/>
-    </row>
-    <row r="66" spans="2:10" s="4" customFormat="1">
+      <c r="K65" s="52"/>
+    </row>
+    <row r="66" spans="2:11" s="4" customFormat="1">
       <c r="B66" s="22"/>
       <c r="C66" s="5"/>
       <c r="D66" s="27"/>
@@ -2452,8 +2848,9 @@
       <c r="H66" s="7"/>
       <c r="I66" s="7"/>
       <c r="J66" s="7"/>
-    </row>
-    <row r="67" spans="2:10" s="4" customFormat="1">
+      <c r="K66" s="52"/>
+    </row>
+    <row r="67" spans="2:11" s="4" customFormat="1">
       <c r="B67" s="22"/>
       <c r="C67" s="5"/>
       <c r="D67" s="27"/>
@@ -2463,8 +2860,9 @@
       <c r="H67" s="7"/>
       <c r="I67" s="7"/>
       <c r="J67" s="7"/>
-    </row>
-    <row r="68" spans="2:10" s="4" customFormat="1">
+      <c r="K67" s="52"/>
+    </row>
+    <row r="68" spans="2:11" s="4" customFormat="1">
       <c r="B68" s="22"/>
       <c r="C68" s="5"/>
       <c r="D68" s="27"/>
@@ -2474,8 +2872,9 @@
       <c r="H68" s="7"/>
       <c r="I68" s="7"/>
       <c r="J68" s="7"/>
-    </row>
-    <row r="69" spans="2:10" s="4" customFormat="1">
+      <c r="K68" s="52"/>
+    </row>
+    <row r="69" spans="2:11" s="4" customFormat="1">
       <c r="B69" s="22"/>
       <c r="C69" s="5"/>
       <c r="D69" s="27"/>
@@ -2485,8 +2884,9 @@
       <c r="H69" s="7"/>
       <c r="I69" s="7"/>
       <c r="J69" s="7"/>
-    </row>
-    <row r="70" spans="2:10" s="4" customFormat="1">
+      <c r="K69" s="52"/>
+    </row>
+    <row r="70" spans="2:11" s="4" customFormat="1">
       <c r="B70" s="22"/>
       <c r="C70" s="5"/>
       <c r="D70" s="27"/>
@@ -2496,8 +2896,9 @@
       <c r="H70" s="7"/>
       <c r="I70" s="7"/>
       <c r="J70" s="7"/>
-    </row>
-    <row r="71" spans="2:10" s="4" customFormat="1">
+      <c r="K70" s="52"/>
+    </row>
+    <row r="71" spans="2:11" s="4" customFormat="1">
       <c r="B71" s="22"/>
       <c r="C71" s="5"/>
       <c r="D71" s="27"/>
@@ -2507,8 +2908,9 @@
       <c r="H71" s="7"/>
       <c r="I71" s="7"/>
       <c r="J71" s="7"/>
-    </row>
-    <row r="72" spans="2:10" s="4" customFormat="1">
+      <c r="K71" s="52"/>
+    </row>
+    <row r="72" spans="2:11" s="4" customFormat="1">
       <c r="B72" s="22"/>
       <c r="C72" s="5"/>
       <c r="D72" s="27"/>
@@ -2518,8 +2920,9 @@
       <c r="H72" s="7"/>
       <c r="I72" s="7"/>
       <c r="J72" s="7"/>
-    </row>
-    <row r="73" spans="2:10" s="4" customFormat="1">
+      <c r="K72" s="52"/>
+    </row>
+    <row r="73" spans="2:11" s="4" customFormat="1">
       <c r="B73" s="22"/>
       <c r="C73" s="5"/>
       <c r="D73" s="27"/>
@@ -2529,8 +2932,9 @@
       <c r="H73" s="7"/>
       <c r="I73" s="7"/>
       <c r="J73" s="7"/>
-    </row>
-    <row r="74" spans="2:10" s="4" customFormat="1">
+      <c r="K73" s="52"/>
+    </row>
+    <row r="74" spans="2:11" s="4" customFormat="1">
       <c r="B74" s="22"/>
       <c r="C74" s="5"/>
       <c r="D74" s="27"/>
@@ -2540,8 +2944,9 @@
       <c r="H74" s="7"/>
       <c r="I74" s="7"/>
       <c r="J74" s="7"/>
-    </row>
-    <row r="75" spans="2:10" s="4" customFormat="1">
+      <c r="K74" s="52"/>
+    </row>
+    <row r="75" spans="2:11" s="4" customFormat="1">
       <c r="B75" s="22"/>
       <c r="C75" s="5"/>
       <c r="D75" s="27"/>
@@ -2551,8 +2956,9 @@
       <c r="H75" s="7"/>
       <c r="I75" s="7"/>
       <c r="J75" s="7"/>
-    </row>
-    <row r="76" spans="2:10" s="4" customFormat="1">
+      <c r="K75" s="52"/>
+    </row>
+    <row r="76" spans="2:11" s="4" customFormat="1">
       <c r="B76" s="22"/>
       <c r="C76" s="5"/>
       <c r="D76" s="27"/>
@@ -2562,8 +2968,9 @@
       <c r="H76" s="7"/>
       <c r="I76" s="7"/>
       <c r="J76" s="7"/>
-    </row>
-    <row r="77" spans="2:10" s="4" customFormat="1">
+      <c r="K76" s="52"/>
+    </row>
+    <row r="77" spans="2:11" s="4" customFormat="1">
       <c r="B77" s="22"/>
       <c r="C77" s="5"/>
       <c r="D77" s="27"/>
@@ -2573,8 +2980,9 @@
       <c r="H77" s="7"/>
       <c r="I77" s="7"/>
       <c r="J77" s="7"/>
-    </row>
-    <row r="78" spans="2:10" s="4" customFormat="1">
+      <c r="K77" s="52"/>
+    </row>
+    <row r="78" spans="2:11" s="4" customFormat="1">
       <c r="B78" s="22"/>
       <c r="C78" s="5"/>
       <c r="D78" s="27"/>
@@ -2584,8 +2992,9 @@
       <c r="H78" s="7"/>
       <c r="I78" s="7"/>
       <c r="J78" s="7"/>
-    </row>
-    <row r="79" spans="2:10" s="4" customFormat="1">
+      <c r="K78" s="52"/>
+    </row>
+    <row r="79" spans="2:11" s="4" customFormat="1">
       <c r="B79" s="22"/>
       <c r="C79" s="5"/>
       <c r="D79" s="27"/>
@@ -2595,8 +3004,9 @@
       <c r="H79" s="7"/>
       <c r="I79" s="7"/>
       <c r="J79" s="7"/>
-    </row>
-    <row r="80" spans="2:10" s="4" customFormat="1">
+      <c r="K79" s="52"/>
+    </row>
+    <row r="80" spans="2:11" s="4" customFormat="1">
       <c r="B80" s="22"/>
       <c r="C80" s="5"/>
       <c r="D80" s="27"/>
@@ -2606,8 +3016,9 @@
       <c r="H80" s="7"/>
       <c r="I80" s="7"/>
       <c r="J80" s="7"/>
-    </row>
-    <row r="81" spans="2:10" s="4" customFormat="1">
+      <c r="K80" s="52"/>
+    </row>
+    <row r="81" spans="2:11" s="4" customFormat="1">
       <c r="B81" s="22"/>
       <c r="C81" s="5"/>
       <c r="D81" s="27"/>
@@ -2617,8 +3028,9 @@
       <c r="H81" s="7"/>
       <c r="I81" s="7"/>
       <c r="J81" s="7"/>
-    </row>
-    <row r="82" spans="2:10" s="4" customFormat="1">
+      <c r="K81" s="52"/>
+    </row>
+    <row r="82" spans="2:11" s="4" customFormat="1">
       <c r="B82" s="22"/>
       <c r="C82" s="5"/>
       <c r="D82" s="27"/>
@@ -2628,8 +3040,9 @@
       <c r="H82" s="7"/>
       <c r="I82" s="7"/>
       <c r="J82" s="7"/>
-    </row>
-    <row r="83" spans="2:10" s="4" customFormat="1">
+      <c r="K82" s="52"/>
+    </row>
+    <row r="83" spans="2:11" s="4" customFormat="1">
       <c r="B83" s="22"/>
       <c r="C83" s="5"/>
       <c r="D83" s="27"/>
@@ -2639,8 +3052,9 @@
       <c r="H83" s="7"/>
       <c r="I83" s="7"/>
       <c r="J83" s="7"/>
-    </row>
-    <row r="84" spans="2:10" s="4" customFormat="1">
+      <c r="K83" s="52"/>
+    </row>
+    <row r="84" spans="2:11" s="4" customFormat="1">
       <c r="B84" s="22"/>
       <c r="C84" s="5"/>
       <c r="D84" s="27"/>
@@ -2650,8 +3064,9 @@
       <c r="H84" s="7"/>
       <c r="I84" s="7"/>
       <c r="J84" s="7"/>
-    </row>
-    <row r="85" spans="2:10" s="4" customFormat="1">
+      <c r="K84" s="52"/>
+    </row>
+    <row r="85" spans="2:11" s="4" customFormat="1">
       <c r="B85" s="22"/>
       <c r="C85" s="5"/>
       <c r="D85" s="27"/>
@@ -2661,8 +3076,9 @@
       <c r="H85" s="7"/>
       <c r="I85" s="7"/>
       <c r="J85" s="7"/>
-    </row>
-    <row r="86" spans="2:10" s="4" customFormat="1">
+      <c r="K85" s="52"/>
+    </row>
+    <row r="86" spans="2:11" s="4" customFormat="1">
       <c r="B86" s="22"/>
       <c r="C86" s="5"/>
       <c r="D86" s="27"/>
@@ -2672,8 +3088,9 @@
       <c r="H86" s="7"/>
       <c r="I86" s="7"/>
       <c r="J86" s="7"/>
-    </row>
-    <row r="87" spans="2:10" s="4" customFormat="1">
+      <c r="K86" s="52"/>
+    </row>
+    <row r="87" spans="2:11" s="4" customFormat="1">
       <c r="B87" s="22"/>
       <c r="C87" s="5"/>
       <c r="D87" s="27"/>
@@ -2683,8 +3100,9 @@
       <c r="H87" s="7"/>
       <c r="I87" s="7"/>
       <c r="J87" s="7"/>
-    </row>
-    <row r="88" spans="2:10" s="4" customFormat="1">
+      <c r="K87" s="52"/>
+    </row>
+    <row r="88" spans="2:11" s="4" customFormat="1">
       <c r="B88" s="22"/>
       <c r="C88" s="5"/>
       <c r="D88" s="27"/>
@@ -2694,8 +3112,9 @@
       <c r="H88" s="7"/>
       <c r="I88" s="7"/>
       <c r="J88" s="7"/>
-    </row>
-    <row r="89" spans="2:10" s="4" customFormat="1">
+      <c r="K88" s="52"/>
+    </row>
+    <row r="89" spans="2:11" s="4" customFormat="1">
       <c r="B89" s="22"/>
       <c r="C89" s="5"/>
       <c r="D89" s="27"/>
@@ -2705,8 +3124,9 @@
       <c r="H89" s="7"/>
       <c r="I89" s="7"/>
       <c r="J89" s="7"/>
-    </row>
-    <row r="90" spans="2:10" s="4" customFormat="1">
+      <c r="K89" s="52"/>
+    </row>
+    <row r="90" spans="2:11" s="4" customFormat="1">
       <c r="B90" s="22"/>
       <c r="C90" s="5"/>
       <c r="D90" s="27"/>
@@ -2716,8 +3136,9 @@
       <c r="H90" s="7"/>
       <c r="I90" s="7"/>
       <c r="J90" s="7"/>
-    </row>
-    <row r="91" spans="2:10" s="4" customFormat="1">
+      <c r="K90" s="52"/>
+    </row>
+    <row r="91" spans="2:11" s="4" customFormat="1">
       <c r="B91" s="22"/>
       <c r="C91" s="5"/>
       <c r="D91" s="27"/>
@@ -2727,8 +3148,9 @@
       <c r="H91" s="7"/>
       <c r="I91" s="7"/>
       <c r="J91" s="7"/>
-    </row>
-    <row r="92" spans="2:10" s="4" customFormat="1">
+      <c r="K91" s="52"/>
+    </row>
+    <row r="92" spans="2:11" s="4" customFormat="1">
       <c r="B92" s="22"/>
       <c r="C92" s="5"/>
       <c r="D92" s="27"/>
@@ -2738,8 +3160,9 @@
       <c r="H92" s="7"/>
       <c r="I92" s="7"/>
       <c r="J92" s="7"/>
-    </row>
-    <row r="93" spans="2:10" s="4" customFormat="1">
+      <c r="K92" s="52"/>
+    </row>
+    <row r="93" spans="2:11" s="4" customFormat="1">
       <c r="B93" s="22"/>
       <c r="C93" s="5"/>
       <c r="D93" s="27"/>
@@ -2749,8 +3172,9 @@
       <c r="H93" s="7"/>
       <c r="I93" s="7"/>
       <c r="J93" s="7"/>
-    </row>
-    <row r="94" spans="2:10" s="4" customFormat="1">
+      <c r="K93" s="52"/>
+    </row>
+    <row r="94" spans="2:11" s="4" customFormat="1">
       <c r="B94" s="22"/>
       <c r="C94" s="5"/>
       <c r="D94" s="27"/>
@@ -2760,8 +3184,9 @@
       <c r="H94" s="7"/>
       <c r="I94" s="7"/>
       <c r="J94" s="7"/>
-    </row>
-    <row r="95" spans="2:10" s="4" customFormat="1">
+      <c r="K94" s="52"/>
+    </row>
+    <row r="95" spans="2:11" s="4" customFormat="1">
       <c r="B95" s="22"/>
       <c r="C95" s="5"/>
       <c r="D95" s="27"/>
@@ -2771,8 +3196,9 @@
       <c r="H95" s="7"/>
       <c r="I95" s="7"/>
       <c r="J95" s="7"/>
-    </row>
-    <row r="96" spans="2:10" s="4" customFormat="1">
+      <c r="K95" s="52"/>
+    </row>
+    <row r="96" spans="2:11" s="4" customFormat="1">
       <c r="B96" s="22"/>
       <c r="C96" s="5"/>
       <c r="D96" s="27"/>
@@ -2782,8 +3208,9 @@
       <c r="H96" s="7"/>
       <c r="I96" s="7"/>
       <c r="J96" s="7"/>
-    </row>
-    <row r="97" spans="2:10" s="4" customFormat="1">
+      <c r="K96" s="52"/>
+    </row>
+    <row r="97" spans="2:11" s="4" customFormat="1">
       <c r="B97" s="22"/>
       <c r="C97" s="5"/>
       <c r="D97" s="27"/>
@@ -2793,8 +3220,9 @@
       <c r="H97" s="7"/>
       <c r="I97" s="7"/>
       <c r="J97" s="7"/>
-    </row>
-    <row r="98" spans="2:10" s="4" customFormat="1">
+      <c r="K97" s="52"/>
+    </row>
+    <row r="98" spans="2:11" s="4" customFormat="1">
       <c r="B98" s="22"/>
       <c r="C98" s="5"/>
       <c r="D98" s="27"/>
@@ -2804,8 +3232,9 @@
       <c r="H98" s="7"/>
       <c r="I98" s="7"/>
       <c r="J98" s="7"/>
-    </row>
-    <row r="99" spans="2:10" s="4" customFormat="1">
+      <c r="K98" s="52"/>
+    </row>
+    <row r="99" spans="2:11" s="4" customFormat="1">
       <c r="B99" s="22"/>
       <c r="C99" s="5"/>
       <c r="D99" s="27"/>
@@ -2815,8 +3244,9 @@
       <c r="H99" s="7"/>
       <c r="I99" s="7"/>
       <c r="J99" s="7"/>
-    </row>
-    <row r="100" spans="2:10" s="4" customFormat="1">
+      <c r="K99" s="52"/>
+    </row>
+    <row r="100" spans="2:11" s="4" customFormat="1">
       <c r="B100" s="22"/>
       <c r="C100" s="5"/>
       <c r="D100" s="27"/>
@@ -2826,8 +3256,9 @@
       <c r="H100" s="7"/>
       <c r="I100" s="7"/>
       <c r="J100" s="7"/>
-    </row>
-    <row r="101" spans="2:10" s="4" customFormat="1">
+      <c r="K100" s="52"/>
+    </row>
+    <row r="101" spans="2:11" s="4" customFormat="1">
       <c r="B101" s="22"/>
       <c r="C101" s="5"/>
       <c r="D101" s="27"/>
@@ -2837,8 +3268,9 @@
       <c r="H101" s="7"/>
       <c r="I101" s="7"/>
       <c r="J101" s="7"/>
-    </row>
-    <row r="102" spans="2:10" s="4" customFormat="1">
+      <c r="K101" s="52"/>
+    </row>
+    <row r="102" spans="2:11" s="4" customFormat="1">
       <c r="B102" s="22"/>
       <c r="C102" s="5"/>
       <c r="D102" s="27"/>
@@ -2848,8 +3280,9 @@
       <c r="H102" s="7"/>
       <c r="I102" s="7"/>
       <c r="J102" s="7"/>
-    </row>
-    <row r="103" spans="2:10" s="4" customFormat="1">
+      <c r="K102" s="52"/>
+    </row>
+    <row r="103" spans="2:11" s="4" customFormat="1">
       <c r="B103" s="22"/>
       <c r="C103" s="5"/>
       <c r="D103" s="27"/>
@@ -2859,8 +3292,9 @@
       <c r="H103" s="7"/>
       <c r="I103" s="7"/>
       <c r="J103" s="7"/>
-    </row>
-    <row r="104" spans="2:10" s="4" customFormat="1">
+      <c r="K103" s="52"/>
+    </row>
+    <row r="104" spans="2:11" s="4" customFormat="1">
       <c r="B104" s="22"/>
       <c r="C104" s="5"/>
       <c r="D104" s="27"/>
@@ -2870,8 +3304,9 @@
       <c r="H104" s="7"/>
       <c r="I104" s="7"/>
       <c r="J104" s="7"/>
-    </row>
-    <row r="105" spans="2:10" s="4" customFormat="1">
+      <c r="K104" s="52"/>
+    </row>
+    <row r="105" spans="2:11" s="4" customFormat="1">
       <c r="B105" s="22"/>
       <c r="C105" s="5"/>
       <c r="D105" s="27"/>
@@ -2881,8 +3316,9 @@
       <c r="H105" s="7"/>
       <c r="I105" s="7"/>
       <c r="J105" s="7"/>
-    </row>
-    <row r="106" spans="2:10" s="4" customFormat="1">
+      <c r="K105" s="52"/>
+    </row>
+    <row r="106" spans="2:11" s="4" customFormat="1">
       <c r="B106" s="22"/>
       <c r="C106" s="5"/>
       <c r="D106" s="27"/>
@@ -2892,8 +3328,9 @@
       <c r="H106" s="7"/>
       <c r="I106" s="7"/>
       <c r="J106" s="7"/>
-    </row>
-    <row r="107" spans="2:10" s="4" customFormat="1">
+      <c r="K106" s="52"/>
+    </row>
+    <row r="107" spans="2:11" s="4" customFormat="1">
       <c r="B107" s="22"/>
       <c r="C107" s="5"/>
       <c r="D107" s="27"/>
@@ -2903,8 +3340,9 @@
       <c r="H107" s="7"/>
       <c r="I107" s="7"/>
       <c r="J107" s="7"/>
-    </row>
-    <row r="108" spans="2:10" s="4" customFormat="1">
+      <c r="K107" s="52"/>
+    </row>
+    <row r="108" spans="2:11" s="4" customFormat="1">
       <c r="B108" s="22"/>
       <c r="C108" s="5"/>
       <c r="D108" s="27"/>
@@ -2914,8 +3352,9 @@
       <c r="H108" s="7"/>
       <c r="I108" s="7"/>
       <c r="J108" s="7"/>
-    </row>
-    <row r="109" spans="2:10" s="4" customFormat="1">
+      <c r="K108" s="52"/>
+    </row>
+    <row r="109" spans="2:11" s="4" customFormat="1">
       <c r="B109" s="22"/>
       <c r="C109" s="5"/>
       <c r="D109" s="27"/>
@@ -2925,8 +3364,9 @@
       <c r="H109" s="7"/>
       <c r="I109" s="7"/>
       <c r="J109" s="7"/>
-    </row>
-    <row r="110" spans="2:10" s="4" customFormat="1">
+      <c r="K109" s="52"/>
+    </row>
+    <row r="110" spans="2:11" s="4" customFormat="1">
       <c r="B110" s="22"/>
       <c r="C110" s="5"/>
       <c r="D110" s="27"/>
@@ -2936,8 +3376,9 @@
       <c r="H110" s="7"/>
       <c r="I110" s="7"/>
       <c r="J110" s="7"/>
-    </row>
-    <row r="111" spans="2:10" s="4" customFormat="1">
+      <c r="K110" s="52"/>
+    </row>
+    <row r="111" spans="2:11" s="4" customFormat="1">
       <c r="B111" s="22"/>
       <c r="C111" s="5"/>
       <c r="D111" s="27"/>
@@ -2947,8 +3388,9 @@
       <c r="H111" s="7"/>
       <c r="I111" s="7"/>
       <c r="J111" s="7"/>
-    </row>
-    <row r="112" spans="2:10" s="4" customFormat="1">
+      <c r="K111" s="52"/>
+    </row>
+    <row r="112" spans="2:11" s="4" customFormat="1">
       <c r="B112" s="22"/>
       <c r="C112" s="5"/>
       <c r="D112" s="27"/>
@@ -2958,8 +3400,9 @@
       <c r="H112" s="7"/>
       <c r="I112" s="7"/>
       <c r="J112" s="7"/>
-    </row>
-    <row r="113" spans="2:10" s="4" customFormat="1">
+      <c r="K112" s="52"/>
+    </row>
+    <row r="113" spans="2:11" s="4" customFormat="1">
       <c r="B113" s="22"/>
       <c r="C113" s="5"/>
       <c r="D113" s="27"/>
@@ -2969,8 +3412,9 @@
       <c r="H113" s="7"/>
       <c r="I113" s="7"/>
       <c r="J113" s="7"/>
-    </row>
-    <row r="114" spans="2:10" s="4" customFormat="1">
+      <c r="K113" s="52"/>
+    </row>
+    <row r="114" spans="2:11" s="4" customFormat="1">
       <c r="B114" s="22"/>
       <c r="C114" s="5"/>
       <c r="D114" s="27"/>
@@ -2980,8 +3424,9 @@
       <c r="H114" s="7"/>
       <c r="I114" s="7"/>
       <c r="J114" s="7"/>
-    </row>
-    <row r="115" spans="2:10" s="4" customFormat="1">
+      <c r="K114" s="52"/>
+    </row>
+    <row r="115" spans="2:11" s="4" customFormat="1">
       <c r="B115" s="22"/>
       <c r="C115" s="5"/>
       <c r="D115" s="27"/>
@@ -2991,8 +3436,9 @@
       <c r="H115" s="7"/>
       <c r="I115" s="7"/>
       <c r="J115" s="7"/>
-    </row>
-    <row r="116" spans="2:10" s="4" customFormat="1">
+      <c r="K115" s="52"/>
+    </row>
+    <row r="116" spans="2:11" s="4" customFormat="1">
       <c r="B116" s="22"/>
       <c r="C116" s="5"/>
       <c r="D116" s="27"/>
@@ -3002,8 +3448,9 @@
       <c r="H116" s="7"/>
       <c r="I116" s="7"/>
       <c r="J116" s="7"/>
-    </row>
-    <row r="117" spans="2:10" s="4" customFormat="1">
+      <c r="K116" s="52"/>
+    </row>
+    <row r="117" spans="2:11" s="4" customFormat="1">
       <c r="B117" s="22"/>
       <c r="C117" s="5"/>
       <c r="D117" s="27"/>
@@ -3013,8 +3460,9 @@
       <c r="H117" s="7"/>
       <c r="I117" s="7"/>
       <c r="J117" s="7"/>
-    </row>
-    <row r="118" spans="2:10" s="4" customFormat="1">
+      <c r="K117" s="52"/>
+    </row>
+    <row r="118" spans="2:11" s="4" customFormat="1">
       <c r="B118" s="22"/>
       <c r="C118" s="5"/>
       <c r="D118" s="27"/>
@@ -3024,8 +3472,9 @@
       <c r="H118" s="7"/>
       <c r="I118" s="7"/>
       <c r="J118" s="7"/>
-    </row>
-    <row r="119" spans="2:10" s="4" customFormat="1">
+      <c r="K118" s="52"/>
+    </row>
+    <row r="119" spans="2:11" s="4" customFormat="1">
       <c r="B119" s="22"/>
       <c r="C119" s="5"/>
       <c r="D119" s="27"/>
@@ -3035,8 +3484,9 @@
       <c r="H119" s="7"/>
       <c r="I119" s="7"/>
       <c r="J119" s="7"/>
-    </row>
-    <row r="120" spans="2:10" s="4" customFormat="1">
+      <c r="K119" s="52"/>
+    </row>
+    <row r="120" spans="2:11" s="4" customFormat="1">
       <c r="B120" s="22"/>
       <c r="C120" s="5"/>
       <c r="D120" s="27"/>
@@ -3046,8 +3496,9 @@
       <c r="H120" s="7"/>
       <c r="I120" s="7"/>
       <c r="J120" s="7"/>
-    </row>
-    <row r="121" spans="2:10" s="4" customFormat="1">
+      <c r="K120" s="52"/>
+    </row>
+    <row r="121" spans="2:11" s="4" customFormat="1">
       <c r="B121" s="22"/>
       <c r="C121" s="5"/>
       <c r="D121" s="27"/>
@@ -3057,8 +3508,9 @@
       <c r="H121" s="7"/>
       <c r="I121" s="7"/>
       <c r="J121" s="7"/>
-    </row>
-    <row r="122" spans="2:10" s="4" customFormat="1">
+      <c r="K121" s="52"/>
+    </row>
+    <row r="122" spans="2:11" s="4" customFormat="1">
       <c r="B122" s="22"/>
       <c r="C122" s="5"/>
       <c r="D122" s="27"/>
@@ -3068,8 +3520,9 @@
       <c r="H122" s="7"/>
       <c r="I122" s="7"/>
       <c r="J122" s="7"/>
-    </row>
-    <row r="123" spans="2:10" s="4" customFormat="1">
+      <c r="K122" s="52"/>
+    </row>
+    <row r="123" spans="2:11" s="4" customFormat="1">
       <c r="B123" s="22"/>
       <c r="C123" s="5"/>
       <c r="D123" s="27"/>
@@ -3079,8 +3532,9 @@
       <c r="H123" s="7"/>
       <c r="I123" s="7"/>
       <c r="J123" s="7"/>
-    </row>
-    <row r="124" spans="2:10" s="4" customFormat="1">
+      <c r="K123" s="52"/>
+    </row>
+    <row r="124" spans="2:11" s="4" customFormat="1">
       <c r="B124" s="22"/>
       <c r="C124" s="5"/>
       <c r="D124" s="27"/>
@@ -3090,8 +3544,9 @@
       <c r="H124" s="7"/>
       <c r="I124" s="7"/>
       <c r="J124" s="7"/>
-    </row>
-    <row r="125" spans="2:10" s="4" customFormat="1">
+      <c r="K124" s="52"/>
+    </row>
+    <row r="125" spans="2:11" s="4" customFormat="1">
       <c r="B125" s="22"/>
       <c r="C125" s="5"/>
       <c r="D125" s="27"/>
@@ -3101,8 +3556,9 @@
       <c r="H125" s="7"/>
       <c r="I125" s="7"/>
       <c r="J125" s="7"/>
-    </row>
-    <row r="126" spans="2:10" s="4" customFormat="1">
+      <c r="K125" s="52"/>
+    </row>
+    <row r="126" spans="2:11" s="4" customFormat="1">
       <c r="B126" s="22"/>
       <c r="C126" s="5"/>
       <c r="D126" s="27"/>
@@ -3112,8 +3568,9 @@
       <c r="H126" s="7"/>
       <c r="I126" s="7"/>
       <c r="J126" s="7"/>
-    </row>
-    <row r="127" spans="2:10" s="4" customFormat="1">
+      <c r="K126" s="52"/>
+    </row>
+    <row r="127" spans="2:11" s="4" customFormat="1">
       <c r="B127" s="22"/>
       <c r="C127" s="5"/>
       <c r="D127" s="27"/>
@@ -3123,8 +3580,9 @@
       <c r="H127" s="7"/>
       <c r="I127" s="7"/>
       <c r="J127" s="7"/>
-    </row>
-    <row r="128" spans="2:10" s="4" customFormat="1">
+      <c r="K127" s="52"/>
+    </row>
+    <row r="128" spans="2:11" s="4" customFormat="1">
       <c r="B128" s="22"/>
       <c r="C128" s="5"/>
       <c r="D128" s="27"/>
@@ -3134,8 +3592,9 @@
       <c r="H128" s="7"/>
       <c r="I128" s="7"/>
       <c r="J128" s="7"/>
-    </row>
-    <row r="129" spans="2:10" s="4" customFormat="1">
+      <c r="K128" s="52"/>
+    </row>
+    <row r="129" spans="2:11" s="4" customFormat="1">
       <c r="B129" s="22"/>
       <c r="C129" s="5"/>
       <c r="D129" s="27"/>
@@ -3145,8 +3604,9 @@
       <c r="H129" s="7"/>
       <c r="I129" s="7"/>
       <c r="J129" s="7"/>
-    </row>
-    <row r="130" spans="2:10" s="4" customFormat="1">
+      <c r="K129" s="52"/>
+    </row>
+    <row r="130" spans="2:11" s="4" customFormat="1">
       <c r="B130" s="22"/>
       <c r="C130" s="5"/>
       <c r="D130" s="27"/>
@@ -3156,8 +3616,9 @@
       <c r="H130" s="7"/>
       <c r="I130" s="7"/>
       <c r="J130" s="7"/>
-    </row>
-    <row r="131" spans="2:10" s="4" customFormat="1">
+      <c r="K130" s="52"/>
+    </row>
+    <row r="131" spans="2:11" s="4" customFormat="1">
       <c r="B131" s="22"/>
       <c r="C131" s="5"/>
       <c r="D131" s="27"/>
@@ -3167,8 +3628,9 @@
       <c r="H131" s="7"/>
       <c r="I131" s="7"/>
       <c r="J131" s="7"/>
-    </row>
-    <row r="132" spans="2:10" s="4" customFormat="1">
+      <c r="K131" s="52"/>
+    </row>
+    <row r="132" spans="2:11" s="4" customFormat="1">
       <c r="B132" s="22"/>
       <c r="C132" s="5"/>
       <c r="D132" s="27"/>
@@ -3178,8 +3640,9 @@
       <c r="H132" s="7"/>
       <c r="I132" s="7"/>
       <c r="J132" s="7"/>
-    </row>
-    <row r="133" spans="2:10" s="4" customFormat="1">
+      <c r="K132" s="52"/>
+    </row>
+    <row r="133" spans="2:11" s="4" customFormat="1">
       <c r="B133" s="22"/>
       <c r="C133" s="5"/>
       <c r="D133" s="27"/>
@@ -3189,8 +3652,9 @@
       <c r="H133" s="7"/>
       <c r="I133" s="7"/>
       <c r="J133" s="7"/>
-    </row>
-    <row r="134" spans="2:10" s="4" customFormat="1">
+      <c r="K133" s="52"/>
+    </row>
+    <row r="134" spans="2:11" s="4" customFormat="1">
       <c r="B134" s="22"/>
       <c r="C134" s="5"/>
       <c r="D134" s="27"/>
@@ -3200,8 +3664,9 @@
       <c r="H134" s="7"/>
       <c r="I134" s="7"/>
       <c r="J134" s="7"/>
-    </row>
-    <row r="135" spans="2:10" s="4" customFormat="1">
+      <c r="K134" s="52"/>
+    </row>
+    <row r="135" spans="2:11" s="4" customFormat="1">
       <c r="B135" s="22"/>
       <c r="C135" s="5"/>
       <c r="D135" s="27"/>
@@ -3211,8 +3676,9 @@
       <c r="H135" s="7"/>
       <c r="I135" s="7"/>
       <c r="J135" s="7"/>
-    </row>
-    <row r="136" spans="2:10" s="4" customFormat="1">
+      <c r="K135" s="52"/>
+    </row>
+    <row r="136" spans="2:11" s="4" customFormat="1">
       <c r="B136" s="22"/>
       <c r="C136" s="5"/>
       <c r="D136" s="27"/>
@@ -3222,8 +3688,9 @@
       <c r="H136" s="7"/>
       <c r="I136" s="7"/>
       <c r="J136" s="7"/>
-    </row>
-    <row r="137" spans="2:10" s="4" customFormat="1">
+      <c r="K136" s="52"/>
+    </row>
+    <row r="137" spans="2:11" s="4" customFormat="1">
       <c r="B137" s="22"/>
       <c r="C137" s="5"/>
       <c r="D137" s="27"/>
@@ -3233,8 +3700,9 @@
       <c r="H137" s="7"/>
       <c r="I137" s="7"/>
       <c r="J137" s="7"/>
-    </row>
-    <row r="138" spans="2:10" s="4" customFormat="1">
+      <c r="K137" s="52"/>
+    </row>
+    <row r="138" spans="2:11" s="4" customFormat="1">
       <c r="B138" s="22"/>
       <c r="C138" s="5"/>
       <c r="D138" s="27"/>
@@ -3244,8 +3712,9 @@
       <c r="H138" s="7"/>
       <c r="I138" s="7"/>
       <c r="J138" s="7"/>
-    </row>
-    <row r="139" spans="2:10" s="4" customFormat="1">
+      <c r="K138" s="52"/>
+    </row>
+    <row r="139" spans="2:11" s="4" customFormat="1">
       <c r="B139" s="22"/>
       <c r="C139" s="5"/>
       <c r="D139" s="27"/>
@@ -3255,8 +3724,9 @@
       <c r="H139" s="7"/>
       <c r="I139" s="7"/>
       <c r="J139" s="7"/>
-    </row>
-    <row r="140" spans="2:10" s="4" customFormat="1">
+      <c r="K139" s="52"/>
+    </row>
+    <row r="140" spans="2:11" s="4" customFormat="1">
       <c r="B140" s="22"/>
       <c r="C140" s="5"/>
       <c r="D140" s="27"/>
@@ -3266,8 +3736,9 @@
       <c r="H140" s="7"/>
       <c r="I140" s="7"/>
       <c r="J140" s="7"/>
-    </row>
-    <row r="141" spans="2:10" s="4" customFormat="1">
+      <c r="K140" s="52"/>
+    </row>
+    <row r="141" spans="2:11" s="4" customFormat="1">
       <c r="B141" s="22"/>
       <c r="C141" s="5"/>
       <c r="D141" s="27"/>
@@ -3277,8 +3748,9 @@
       <c r="H141" s="7"/>
       <c r="I141" s="7"/>
       <c r="J141" s="7"/>
-    </row>
-    <row r="142" spans="2:10" s="4" customFormat="1">
+      <c r="K141" s="52"/>
+    </row>
+    <row r="142" spans="2:11" s="4" customFormat="1">
       <c r="B142" s="22"/>
       <c r="C142" s="5"/>
       <c r="D142" s="27"/>
@@ -3288,8 +3760,9 @@
       <c r="H142" s="7"/>
       <c r="I142" s="7"/>
       <c r="J142" s="7"/>
-    </row>
-    <row r="143" spans="2:10" s="4" customFormat="1">
+      <c r="K142" s="52"/>
+    </row>
+    <row r="143" spans="2:11" s="4" customFormat="1">
       <c r="B143" s="22"/>
       <c r="C143" s="5"/>
       <c r="D143" s="27"/>
@@ -3299,8 +3772,9 @@
       <c r="H143" s="7"/>
       <c r="I143" s="7"/>
       <c r="J143" s="7"/>
-    </row>
-    <row r="144" spans="2:10" s="4" customFormat="1">
+      <c r="K143" s="52"/>
+    </row>
+    <row r="144" spans="2:11" s="4" customFormat="1">
       <c r="B144" s="22"/>
       <c r="C144" s="5"/>
       <c r="D144" s="27"/>
@@ -3310,8 +3784,9 @@
       <c r="H144" s="7"/>
       <c r="I144" s="7"/>
       <c r="J144" s="7"/>
-    </row>
-    <row r="145" spans="2:10" s="4" customFormat="1">
+      <c r="K144" s="52"/>
+    </row>
+    <row r="145" spans="2:11" s="4" customFormat="1">
       <c r="B145" s="22"/>
       <c r="C145" s="5"/>
       <c r="D145" s="27"/>
@@ -3321,8 +3796,9 @@
       <c r="H145" s="7"/>
       <c r="I145" s="7"/>
       <c r="J145" s="7"/>
-    </row>
-    <row r="146" spans="2:10" s="4" customFormat="1">
+      <c r="K145" s="52"/>
+    </row>
+    <row r="146" spans="2:11" s="4" customFormat="1">
       <c r="B146" s="22"/>
       <c r="C146" s="5"/>
       <c r="D146" s="27"/>
@@ -3332,8 +3808,9 @@
       <c r="H146" s="7"/>
       <c r="I146" s="7"/>
       <c r="J146" s="7"/>
-    </row>
-    <row r="147" spans="2:10" s="4" customFormat="1">
+      <c r="K146" s="52"/>
+    </row>
+    <row r="147" spans="2:11" s="4" customFormat="1">
       <c r="B147" s="22"/>
       <c r="C147" s="5"/>
       <c r="D147" s="27"/>
@@ -3343,8 +3820,9 @@
       <c r="H147" s="7"/>
       <c r="I147" s="7"/>
       <c r="J147" s="7"/>
-    </row>
-    <row r="148" spans="2:10" s="4" customFormat="1">
+      <c r="K147" s="52"/>
+    </row>
+    <row r="148" spans="2:11" s="4" customFormat="1">
       <c r="B148" s="22"/>
       <c r="C148" s="5"/>
       <c r="D148" s="27"/>
@@ -3354,8 +3832,9 @@
       <c r="H148" s="7"/>
       <c r="I148" s="7"/>
       <c r="J148" s="7"/>
-    </row>
-    <row r="149" spans="2:10" s="4" customFormat="1">
+      <c r="K148" s="52"/>
+    </row>
+    <row r="149" spans="2:11" s="4" customFormat="1">
       <c r="B149" s="22"/>
       <c r="C149" s="5"/>
       <c r="D149" s="27"/>
@@ -3365,8 +3844,9 @@
       <c r="H149" s="7"/>
       <c r="I149" s="7"/>
       <c r="J149" s="7"/>
-    </row>
-    <row r="150" spans="2:10" s="4" customFormat="1">
+      <c r="K149" s="52"/>
+    </row>
+    <row r="150" spans="2:11" s="4" customFormat="1">
       <c r="B150" s="22"/>
       <c r="C150" s="5"/>
       <c r="D150" s="27"/>
@@ -3376,8 +3856,9 @@
       <c r="H150" s="7"/>
       <c r="I150" s="7"/>
       <c r="J150" s="7"/>
-    </row>
-    <row r="151" spans="2:10" s="4" customFormat="1">
+      <c r="K150" s="52"/>
+    </row>
+    <row r="151" spans="2:11" s="4" customFormat="1">
       <c r="B151" s="22"/>
       <c r="C151" s="5"/>
       <c r="D151" s="27"/>
@@ -3387,8 +3868,9 @@
       <c r="H151" s="7"/>
       <c r="I151" s="7"/>
       <c r="J151" s="7"/>
-    </row>
-    <row r="152" spans="2:10" s="4" customFormat="1">
+      <c r="K151" s="52"/>
+    </row>
+    <row r="152" spans="2:11" s="4" customFormat="1">
       <c r="B152" s="22"/>
       <c r="C152" s="5"/>
       <c r="D152" s="27"/>
@@ -3398,8 +3880,9 @@
       <c r="H152" s="7"/>
       <c r="I152" s="7"/>
       <c r="J152" s="7"/>
-    </row>
-    <row r="153" spans="2:10" s="4" customFormat="1">
+      <c r="K152" s="52"/>
+    </row>
+    <row r="153" spans="2:11" s="4" customFormat="1">
       <c r="B153" s="22"/>
       <c r="C153" s="5"/>
       <c r="D153" s="27"/>
@@ -3409,8 +3892,9 @@
       <c r="H153" s="7"/>
       <c r="I153" s="7"/>
       <c r="J153" s="7"/>
-    </row>
-    <row r="154" spans="2:10" s="4" customFormat="1">
+      <c r="K153" s="52"/>
+    </row>
+    <row r="154" spans="2:11" s="4" customFormat="1">
       <c r="B154" s="22"/>
       <c r="C154" s="5"/>
       <c r="D154" s="27"/>
@@ -3420,8 +3904,9 @@
       <c r="H154" s="7"/>
       <c r="I154" s="7"/>
       <c r="J154" s="7"/>
-    </row>
-    <row r="155" spans="2:10" s="4" customFormat="1">
+      <c r="K154" s="52"/>
+    </row>
+    <row r="155" spans="2:11" s="4" customFormat="1">
       <c r="B155" s="22"/>
       <c r="C155" s="5"/>
       <c r="D155" s="27"/>
@@ -3431,8 +3916,9 @@
       <c r="H155" s="7"/>
       <c r="I155" s="7"/>
       <c r="J155" s="7"/>
-    </row>
-    <row r="156" spans="2:10" s="4" customFormat="1">
+      <c r="K155" s="52"/>
+    </row>
+    <row r="156" spans="2:11" s="4" customFormat="1">
       <c r="B156" s="22"/>
       <c r="C156" s="5"/>
       <c r="D156" s="27"/>
@@ -3442,8 +3928,9 @@
       <c r="H156" s="7"/>
       <c r="I156" s="7"/>
       <c r="J156" s="7"/>
-    </row>
-    <row r="157" spans="2:10" s="4" customFormat="1">
+      <c r="K156" s="52"/>
+    </row>
+    <row r="157" spans="2:11" s="4" customFormat="1">
       <c r="B157" s="22"/>
       <c r="C157" s="5"/>
       <c r="D157" s="27"/>
@@ -3453,8 +3940,9 @@
       <c r="H157" s="7"/>
       <c r="I157" s="7"/>
       <c r="J157" s="7"/>
-    </row>
-    <row r="158" spans="2:10" s="4" customFormat="1">
+      <c r="K157" s="52"/>
+    </row>
+    <row r="158" spans="2:11" s="4" customFormat="1">
       <c r="B158" s="22"/>
       <c r="C158" s="5"/>
       <c r="D158" s="27"/>
@@ -3464,8 +3952,9 @@
       <c r="H158" s="7"/>
       <c r="I158" s="7"/>
       <c r="J158" s="7"/>
-    </row>
-    <row r="159" spans="2:10" s="4" customFormat="1">
+      <c r="K158" s="52"/>
+    </row>
+    <row r="159" spans="2:11" s="4" customFormat="1">
       <c r="B159" s="22"/>
       <c r="C159" s="5"/>
       <c r="D159" s="27"/>
@@ -3475,8 +3964,9 @@
       <c r="H159" s="7"/>
       <c r="I159" s="7"/>
       <c r="J159" s="7"/>
-    </row>
-    <row r="160" spans="2:10" s="4" customFormat="1">
+      <c r="K159" s="52"/>
+    </row>
+    <row r="160" spans="2:11" s="4" customFormat="1">
       <c r="B160" s="22"/>
       <c r="C160" s="5"/>
       <c r="D160" s="27"/>
@@ -3486,8 +3976,9 @@
       <c r="H160" s="7"/>
       <c r="I160" s="7"/>
       <c r="J160" s="7"/>
-    </row>
-    <row r="161" spans="2:10" s="4" customFormat="1">
+      <c r="K160" s="52"/>
+    </row>
+    <row r="161" spans="2:11" s="4" customFormat="1">
       <c r="B161" s="22"/>
       <c r="C161" s="5"/>
       <c r="D161" s="27"/>
@@ -3497,8 +3988,9 @@
       <c r="H161" s="7"/>
       <c r="I161" s="7"/>
       <c r="J161" s="7"/>
-    </row>
-    <row r="162" spans="2:10" s="4" customFormat="1">
+      <c r="K161" s="52"/>
+    </row>
+    <row r="162" spans="2:11" s="4" customFormat="1">
       <c r="B162" s="22"/>
       <c r="C162" s="5"/>
       <c r="D162" s="27"/>
@@ -3508,8 +4000,9 @@
       <c r="H162" s="7"/>
       <c r="I162" s="7"/>
       <c r="J162" s="7"/>
-    </row>
-    <row r="163" spans="2:10" s="4" customFormat="1">
+      <c r="K162" s="52"/>
+    </row>
+    <row r="163" spans="2:11" s="4" customFormat="1">
       <c r="B163" s="22"/>
       <c r="C163" s="5"/>
       <c r="D163" s="27"/>
@@ -3519,8 +4012,9 @@
       <c r="H163" s="7"/>
       <c r="I163" s="7"/>
       <c r="J163" s="7"/>
-    </row>
-    <row r="164" spans="2:10" s="4" customFormat="1">
+      <c r="K163" s="52"/>
+    </row>
+    <row r="164" spans="2:11" s="4" customFormat="1">
       <c r="B164" s="22"/>
       <c r="C164" s="5"/>
       <c r="D164" s="27"/>
@@ -3530,8 +4024,9 @@
       <c r="H164" s="7"/>
       <c r="I164" s="7"/>
       <c r="J164" s="7"/>
-    </row>
-    <row r="165" spans="2:10" s="4" customFormat="1">
+      <c r="K164" s="52"/>
+    </row>
+    <row r="165" spans="2:11" s="4" customFormat="1">
       <c r="B165" s="22"/>
       <c r="C165" s="5"/>
       <c r="D165" s="27"/>
@@ -3541,8 +4036,9 @@
       <c r="H165" s="7"/>
       <c r="I165" s="7"/>
       <c r="J165" s="7"/>
-    </row>
-    <row r="166" spans="2:10" s="4" customFormat="1">
+      <c r="K165" s="52"/>
+    </row>
+    <row r="166" spans="2:11" s="4" customFormat="1">
       <c r="B166" s="22"/>
       <c r="C166" s="5"/>
       <c r="D166" s="27"/>
@@ -3552,8 +4048,9 @@
       <c r="H166" s="7"/>
       <c r="I166" s="7"/>
       <c r="J166" s="7"/>
-    </row>
-    <row r="167" spans="2:10" s="4" customFormat="1">
+      <c r="K166" s="52"/>
+    </row>
+    <row r="167" spans="2:11" s="4" customFormat="1">
       <c r="B167" s="22"/>
       <c r="C167" s="5"/>
       <c r="D167" s="27"/>
@@ -3563,8 +4060,9 @@
       <c r="H167" s="7"/>
       <c r="I167" s="7"/>
       <c r="J167" s="7"/>
-    </row>
-    <row r="168" spans="2:10" s="4" customFormat="1">
+      <c r="K167" s="52"/>
+    </row>
+    <row r="168" spans="2:11" s="4" customFormat="1">
       <c r="B168" s="22"/>
       <c r="C168" s="5"/>
       <c r="D168" s="27"/>
@@ -3574,8 +4072,9 @@
       <c r="H168" s="7"/>
       <c r="I168" s="7"/>
       <c r="J168" s="7"/>
-    </row>
-    <row r="169" spans="2:10" s="4" customFormat="1">
+      <c r="K168" s="52"/>
+    </row>
+    <row r="169" spans="2:11" s="4" customFormat="1">
       <c r="B169" s="22"/>
       <c r="C169" s="5"/>
       <c r="D169" s="27"/>
@@ -3585,8 +4084,9 @@
       <c r="H169" s="7"/>
       <c r="I169" s="7"/>
       <c r="J169" s="7"/>
-    </row>
-    <row r="170" spans="2:10" s="4" customFormat="1">
+      <c r="K169" s="52"/>
+    </row>
+    <row r="170" spans="2:11" s="4" customFormat="1">
       <c r="B170" s="22"/>
       <c r="C170" s="5"/>
       <c r="D170" s="27"/>
@@ -3596,8 +4096,9 @@
       <c r="H170" s="7"/>
       <c r="I170" s="7"/>
       <c r="J170" s="7"/>
-    </row>
-    <row r="171" spans="2:10" s="4" customFormat="1">
+      <c r="K170" s="52"/>
+    </row>
+    <row r="171" spans="2:11" s="4" customFormat="1">
       <c r="B171" s="22"/>
       <c r="C171" s="5"/>
       <c r="D171" s="27"/>
@@ -3607,8 +4108,9 @@
       <c r="H171" s="7"/>
       <c r="I171" s="7"/>
       <c r="J171" s="7"/>
-    </row>
-    <row r="172" spans="2:10" s="4" customFormat="1">
+      <c r="K171" s="52"/>
+    </row>
+    <row r="172" spans="2:11" s="4" customFormat="1">
       <c r="B172" s="22"/>
       <c r="C172" s="5"/>
       <c r="D172" s="27"/>
@@ -3618,8 +4120,9 @@
       <c r="H172" s="7"/>
       <c r="I172" s="7"/>
       <c r="J172" s="7"/>
-    </row>
-    <row r="173" spans="2:10" s="4" customFormat="1">
+      <c r="K172" s="52"/>
+    </row>
+    <row r="173" spans="2:11" s="4" customFormat="1">
       <c r="B173" s="22"/>
       <c r="C173" s="5"/>
       <c r="D173" s="27"/>
@@ -3629,8 +4132,9 @@
       <c r="H173" s="7"/>
       <c r="I173" s="7"/>
       <c r="J173" s="7"/>
-    </row>
-    <row r="174" spans="2:10" s="4" customFormat="1">
+      <c r="K173" s="52"/>
+    </row>
+    <row r="174" spans="2:11" s="4" customFormat="1">
       <c r="B174" s="22"/>
       <c r="C174" s="5"/>
       <c r="D174" s="27"/>
@@ -3640,8 +4144,9 @@
       <c r="H174" s="7"/>
       <c r="I174" s="7"/>
       <c r="J174" s="7"/>
-    </row>
-    <row r="175" spans="2:10" s="4" customFormat="1">
+      <c r="K174" s="52"/>
+    </row>
+    <row r="175" spans="2:11" s="4" customFormat="1">
       <c r="B175" s="22"/>
       <c r="C175" s="5"/>
       <c r="D175" s="27"/>
@@ -3651,8 +4156,9 @@
       <c r="H175" s="7"/>
       <c r="I175" s="7"/>
       <c r="J175" s="7"/>
-    </row>
-    <row r="176" spans="2:10" s="4" customFormat="1">
+      <c r="K175" s="52"/>
+    </row>
+    <row r="176" spans="2:11" s="4" customFormat="1">
       <c r="B176" s="22"/>
       <c r="C176" s="5"/>
       <c r="D176" s="27"/>
@@ -3662,8 +4168,9 @@
       <c r="H176" s="7"/>
       <c r="I176" s="7"/>
       <c r="J176" s="7"/>
-    </row>
-    <row r="177" spans="2:10" s="4" customFormat="1">
+      <c r="K176" s="52"/>
+    </row>
+    <row r="177" spans="2:11" s="4" customFormat="1">
       <c r="B177" s="22"/>
       <c r="C177" s="5"/>
       <c r="D177" s="27"/>
@@ -3673,8 +4180,9 @@
       <c r="H177" s="7"/>
       <c r="I177" s="7"/>
       <c r="J177" s="7"/>
-    </row>
-    <row r="178" spans="2:10" s="4" customFormat="1">
+      <c r="K177" s="52"/>
+    </row>
+    <row r="178" spans="2:11" s="4" customFormat="1">
       <c r="B178" s="22"/>
       <c r="C178" s="5"/>
       <c r="D178" s="27"/>
@@ -3684,8 +4192,9 @@
       <c r="H178" s="7"/>
       <c r="I178" s="7"/>
       <c r="J178" s="7"/>
-    </row>
-    <row r="179" spans="2:10" s="4" customFormat="1">
+      <c r="K178" s="52"/>
+    </row>
+    <row r="179" spans="2:11" s="4" customFormat="1">
       <c r="B179" s="22"/>
       <c r="C179" s="5"/>
       <c r="D179" s="27"/>
@@ -3695,8 +4204,9 @@
       <c r="H179" s="7"/>
       <c r="I179" s="7"/>
       <c r="J179" s="7"/>
-    </row>
-    <row r="180" spans="2:10" s="4" customFormat="1">
+      <c r="K179" s="52"/>
+    </row>
+    <row r="180" spans="2:11" s="4" customFormat="1">
       <c r="B180" s="22"/>
       <c r="C180" s="5"/>
       <c r="D180" s="27"/>
@@ -3706,8 +4216,9 @@
       <c r="H180" s="7"/>
       <c r="I180" s="7"/>
       <c r="J180" s="7"/>
-    </row>
-    <row r="181" spans="2:10" s="4" customFormat="1">
+      <c r="K180" s="52"/>
+    </row>
+    <row r="181" spans="2:11" s="4" customFormat="1">
       <c r="B181" s="22"/>
       <c r="C181" s="5"/>
       <c r="D181" s="27"/>
@@ -3717,8 +4228,9 @@
       <c r="H181" s="7"/>
       <c r="I181" s="7"/>
       <c r="J181" s="7"/>
-    </row>
-    <row r="182" spans="2:10" s="4" customFormat="1">
+      <c r="K181" s="52"/>
+    </row>
+    <row r="182" spans="2:11" s="4" customFormat="1">
       <c r="B182" s="22"/>
       <c r="C182" s="5"/>
       <c r="D182" s="27"/>
@@ -3728,8 +4240,9 @@
       <c r="H182" s="7"/>
       <c r="I182" s="7"/>
       <c r="J182" s="7"/>
-    </row>
-    <row r="183" spans="2:10" s="4" customFormat="1">
+      <c r="K182" s="52"/>
+    </row>
+    <row r="183" spans="2:11" s="4" customFormat="1">
       <c r="B183" s="22"/>
       <c r="C183" s="5"/>
       <c r="D183" s="27"/>
@@ -3739,8 +4252,9 @@
       <c r="H183" s="7"/>
       <c r="I183" s="7"/>
       <c r="J183" s="7"/>
-    </row>
-    <row r="184" spans="2:10" s="4" customFormat="1">
+      <c r="K183" s="52"/>
+    </row>
+    <row r="184" spans="2:11" s="4" customFormat="1">
       <c r="B184" s="22"/>
       <c r="C184" s="5"/>
       <c r="D184" s="27"/>
@@ -3750,8 +4264,9 @@
       <c r="H184" s="7"/>
       <c r="I184" s="7"/>
       <c r="J184" s="7"/>
-    </row>
-    <row r="185" spans="2:10" s="4" customFormat="1">
+      <c r="K184" s="52"/>
+    </row>
+    <row r="185" spans="2:11" s="4" customFormat="1">
       <c r="B185" s="22"/>
       <c r="C185" s="5"/>
       <c r="D185" s="27"/>
@@ -3761,8 +4276,9 @@
       <c r="H185" s="7"/>
       <c r="I185" s="7"/>
       <c r="J185" s="7"/>
-    </row>
-    <row r="186" spans="2:10" s="4" customFormat="1">
+      <c r="K185" s="52"/>
+    </row>
+    <row r="186" spans="2:11" s="4" customFormat="1">
       <c r="B186" s="22"/>
       <c r="C186" s="5"/>
       <c r="D186" s="27"/>
@@ -3772,8 +4288,9 @@
       <c r="H186" s="7"/>
       <c r="I186" s="7"/>
       <c r="J186" s="7"/>
-    </row>
-    <row r="187" spans="2:10" s="4" customFormat="1">
+      <c r="K186" s="52"/>
+    </row>
+    <row r="187" spans="2:11" s="4" customFormat="1">
       <c r="B187" s="22"/>
       <c r="C187" s="5"/>
       <c r="D187" s="27"/>
@@ -3783,8 +4300,9 @@
       <c r="H187" s="7"/>
       <c r="I187" s="7"/>
       <c r="J187" s="7"/>
-    </row>
-    <row r="188" spans="2:10" s="4" customFormat="1">
+      <c r="K187" s="52"/>
+    </row>
+    <row r="188" spans="2:11" s="4" customFormat="1">
       <c r="B188" s="22"/>
       <c r="C188" s="5"/>
       <c r="D188" s="27"/>
@@ -3794,8 +4312,9 @@
       <c r="H188" s="7"/>
       <c r="I188" s="7"/>
       <c r="J188" s="7"/>
-    </row>
-    <row r="189" spans="2:10" s="4" customFormat="1">
+      <c r="K188" s="52"/>
+    </row>
+    <row r="189" spans="2:11" s="4" customFormat="1">
       <c r="B189" s="22"/>
       <c r="C189" s="5"/>
       <c r="D189" s="27"/>
@@ -3805,8 +4324,9 @@
       <c r="H189" s="7"/>
       <c r="I189" s="7"/>
       <c r="J189" s="7"/>
-    </row>
-    <row r="190" spans="2:10" s="4" customFormat="1">
+      <c r="K189" s="52"/>
+    </row>
+    <row r="190" spans="2:11" s="4" customFormat="1">
       <c r="B190" s="22"/>
       <c r="C190" s="5"/>
       <c r="D190" s="27"/>
@@ -3816,8 +4336,9 @@
       <c r="H190" s="7"/>
       <c r="I190" s="7"/>
       <c r="J190" s="7"/>
-    </row>
-    <row r="191" spans="2:10" s="4" customFormat="1">
+      <c r="K190" s="52"/>
+    </row>
+    <row r="191" spans="2:11" s="4" customFormat="1">
       <c r="B191" s="22"/>
       <c r="C191" s="5"/>
       <c r="D191" s="27"/>
@@ -3827,8 +4348,9 @@
       <c r="H191" s="7"/>
       <c r="I191" s="7"/>
       <c r="J191" s="7"/>
-    </row>
-    <row r="192" spans="2:10" s="4" customFormat="1">
+      <c r="K191" s="52"/>
+    </row>
+    <row r="192" spans="2:11" s="4" customFormat="1">
       <c r="B192" s="22"/>
       <c r="C192" s="5"/>
       <c r="D192" s="27"/>
@@ -3838,8 +4360,9 @@
       <c r="H192" s="7"/>
       <c r="I192" s="7"/>
       <c r="J192" s="7"/>
-    </row>
-    <row r="193" spans="2:10" s="4" customFormat="1">
+      <c r="K192" s="52"/>
+    </row>
+    <row r="193" spans="2:11" s="4" customFormat="1">
       <c r="B193" s="22"/>
       <c r="C193" s="5"/>
       <c r="D193" s="27"/>
@@ -3849,8 +4372,9 @@
       <c r="H193" s="7"/>
       <c r="I193" s="7"/>
       <c r="J193" s="7"/>
-    </row>
-    <row r="194" spans="2:10" s="4" customFormat="1">
+      <c r="K193" s="52"/>
+    </row>
+    <row r="194" spans="2:11" s="4" customFormat="1">
       <c r="B194" s="22"/>
       <c r="C194" s="5"/>
       <c r="D194" s="27"/>
@@ -3860,8 +4384,9 @@
       <c r="H194" s="7"/>
       <c r="I194" s="7"/>
       <c r="J194" s="7"/>
-    </row>
-    <row r="195" spans="2:10" s="4" customFormat="1">
+      <c r="K194" s="52"/>
+    </row>
+    <row r="195" spans="2:11" s="4" customFormat="1">
       <c r="B195" s="22"/>
       <c r="C195" s="5"/>
       <c r="D195" s="27"/>
@@ -3871,8 +4396,9 @@
       <c r="H195" s="7"/>
       <c r="I195" s="7"/>
       <c r="J195" s="7"/>
-    </row>
-    <row r="196" spans="2:10" s="4" customFormat="1">
+      <c r="K195" s="52"/>
+    </row>
+    <row r="196" spans="2:11" s="4" customFormat="1">
       <c r="B196" s="22"/>
       <c r="C196" s="5"/>
       <c r="D196" s="27"/>
@@ -3882,8 +4408,9 @@
       <c r="H196" s="7"/>
       <c r="I196" s="7"/>
       <c r="J196" s="7"/>
-    </row>
-    <row r="197" spans="2:10" s="4" customFormat="1">
+      <c r="K196" s="52"/>
+    </row>
+    <row r="197" spans="2:11" s="4" customFormat="1">
       <c r="B197" s="22"/>
       <c r="C197" s="5"/>
       <c r="D197" s="27"/>
@@ -3893,8 +4420,9 @@
       <c r="H197" s="7"/>
       <c r="I197" s="7"/>
       <c r="J197" s="7"/>
-    </row>
-    <row r="198" spans="2:10" s="4" customFormat="1">
+      <c r="K197" s="52"/>
+    </row>
+    <row r="198" spans="2:11" s="4" customFormat="1">
       <c r="B198" s="22"/>
       <c r="C198" s="5"/>
       <c r="D198" s="27"/>
@@ -3904,8 +4432,9 @@
       <c r="H198" s="7"/>
       <c r="I198" s="7"/>
       <c r="J198" s="7"/>
-    </row>
-    <row r="199" spans="2:10" s="4" customFormat="1">
+      <c r="K198" s="52"/>
+    </row>
+    <row r="199" spans="2:11" s="4" customFormat="1">
       <c r="B199" s="22"/>
       <c r="C199" s="5"/>
       <c r="D199" s="27"/>
@@ -3915,8 +4444,9 @@
       <c r="H199" s="7"/>
       <c r="I199" s="7"/>
       <c r="J199" s="7"/>
-    </row>
-    <row r="200" spans="2:10" s="4" customFormat="1">
+      <c r="K199" s="52"/>
+    </row>
+    <row r="200" spans="2:11" s="4" customFormat="1">
       <c r="B200" s="22"/>
       <c r="C200" s="5"/>
       <c r="D200" s="27"/>
@@ -3926,8 +4456,9 @@
       <c r="H200" s="7"/>
       <c r="I200" s="7"/>
       <c r="J200" s="7"/>
-    </row>
-    <row r="201" spans="2:10" s="4" customFormat="1">
+      <c r="K200" s="52"/>
+    </row>
+    <row r="201" spans="2:11" s="4" customFormat="1">
       <c r="B201" s="22"/>
       <c r="C201" s="5"/>
       <c r="D201" s="27"/>
@@ -3937,8 +4468,9 @@
       <c r="H201" s="7"/>
       <c r="I201" s="7"/>
       <c r="J201" s="7"/>
-    </row>
-    <row r="202" spans="2:10" s="4" customFormat="1">
+      <c r="K201" s="52"/>
+    </row>
+    <row r="202" spans="2:11" s="4" customFormat="1">
       <c r="B202" s="22"/>
       <c r="C202" s="5"/>
       <c r="D202" s="27"/>
@@ -3948,8 +4480,9 @@
       <c r="H202" s="7"/>
       <c r="I202" s="7"/>
       <c r="J202" s="7"/>
-    </row>
-    <row r="203" spans="2:10" s="4" customFormat="1">
+      <c r="K202" s="52"/>
+    </row>
+    <row r="203" spans="2:11" s="4" customFormat="1">
       <c r="B203" s="22"/>
       <c r="C203" s="5"/>
       <c r="D203" s="27"/>
@@ -3959,8 +4492,9 @@
       <c r="H203" s="7"/>
       <c r="I203" s="7"/>
       <c r="J203" s="7"/>
-    </row>
-    <row r="204" spans="2:10" s="4" customFormat="1">
+      <c r="K203" s="52"/>
+    </row>
+    <row r="204" spans="2:11" s="4" customFormat="1">
       <c r="B204" s="22"/>
       <c r="C204" s="5"/>
       <c r="D204" s="27"/>
@@ -3970,8 +4504,9 @@
       <c r="H204" s="7"/>
       <c r="I204" s="7"/>
       <c r="J204" s="7"/>
-    </row>
-    <row r="205" spans="2:10" s="4" customFormat="1">
+      <c r="K204" s="52"/>
+    </row>
+    <row r="205" spans="2:11" s="4" customFormat="1">
       <c r="B205" s="22"/>
       <c r="C205" s="5"/>
       <c r="D205" s="27"/>
@@ -3981,8 +4516,9 @@
       <c r="H205" s="7"/>
       <c r="I205" s="7"/>
       <c r="J205" s="7"/>
-    </row>
-    <row r="206" spans="2:10" s="4" customFormat="1">
+      <c r="K205" s="52"/>
+    </row>
+    <row r="206" spans="2:11" s="4" customFormat="1">
       <c r="B206" s="22"/>
       <c r="C206" s="5"/>
       <c r="D206" s="27"/>
@@ -3992,8 +4528,9 @@
       <c r="H206" s="7"/>
       <c r="I206" s="7"/>
       <c r="J206" s="7"/>
-    </row>
-    <row r="207" spans="2:10" s="4" customFormat="1">
+      <c r="K206" s="52"/>
+    </row>
+    <row r="207" spans="2:11" s="4" customFormat="1">
       <c r="B207" s="22"/>
       <c r="C207" s="5"/>
       <c r="D207" s="27"/>
@@ -4003,8 +4540,9 @@
       <c r="H207" s="7"/>
       <c r="I207" s="7"/>
       <c r="J207" s="7"/>
-    </row>
-    <row r="208" spans="2:10" s="4" customFormat="1">
+      <c r="K207" s="52"/>
+    </row>
+    <row r="208" spans="2:11" s="4" customFormat="1">
       <c r="B208" s="22"/>
       <c r="C208" s="5"/>
       <c r="D208" s="27"/>
@@ -4014,8 +4552,9 @@
       <c r="H208" s="7"/>
       <c r="I208" s="7"/>
       <c r="J208" s="7"/>
-    </row>
-    <row r="209" spans="2:10" s="4" customFormat="1">
+      <c r="K208" s="52"/>
+    </row>
+    <row r="209" spans="2:11" s="4" customFormat="1">
       <c r="B209" s="22"/>
       <c r="C209" s="5"/>
       <c r="D209" s="27"/>
@@ -4025,8 +4564,9 @@
       <c r="H209" s="7"/>
       <c r="I209" s="7"/>
       <c r="J209" s="7"/>
-    </row>
-    <row r="210" spans="2:10" s="4" customFormat="1">
+      <c r="K209" s="52"/>
+    </row>
+    <row r="210" spans="2:11" s="4" customFormat="1">
       <c r="B210" s="22"/>
       <c r="C210" s="5"/>
       <c r="D210" s="27"/>
@@ -4036,8 +4576,9 @@
       <c r="H210" s="7"/>
       <c r="I210" s="7"/>
       <c r="J210" s="7"/>
-    </row>
-    <row r="211" spans="2:10" s="4" customFormat="1">
+      <c r="K210" s="52"/>
+    </row>
+    <row r="211" spans="2:11" s="4" customFormat="1">
       <c r="B211" s="22"/>
       <c r="C211" s="5"/>
       <c r="D211" s="27"/>
@@ -4047,8 +4588,9 @@
       <c r="H211" s="7"/>
       <c r="I211" s="7"/>
       <c r="J211" s="7"/>
-    </row>
-    <row r="212" spans="2:10" s="4" customFormat="1">
+      <c r="K211" s="52"/>
+    </row>
+    <row r="212" spans="2:11" s="4" customFormat="1">
       <c r="B212" s="22"/>
       <c r="C212" s="5"/>
       <c r="D212" s="27"/>
@@ -4058,8 +4600,9 @@
       <c r="H212" s="7"/>
       <c r="I212" s="7"/>
       <c r="J212" s="7"/>
-    </row>
-    <row r="213" spans="2:10" s="4" customFormat="1">
+      <c r="K212" s="52"/>
+    </row>
+    <row r="213" spans="2:11" s="4" customFormat="1">
       <c r="B213" s="22"/>
       <c r="C213" s="5"/>
       <c r="D213" s="27"/>
@@ -4069,8 +4612,9 @@
       <c r="H213" s="7"/>
       <c r="I213" s="7"/>
       <c r="J213" s="7"/>
-    </row>
-    <row r="214" spans="2:10" s="4" customFormat="1">
+      <c r="K213" s="52"/>
+    </row>
+    <row r="214" spans="2:11" s="4" customFormat="1">
       <c r="B214" s="22"/>
       <c r="C214" s="5"/>
       <c r="D214" s="27"/>
@@ -4080,8 +4624,9 @@
       <c r="H214" s="7"/>
       <c r="I214" s="7"/>
       <c r="J214" s="7"/>
-    </row>
-    <row r="215" spans="2:10" s="4" customFormat="1">
+      <c r="K214" s="52"/>
+    </row>
+    <row r="215" spans="2:11" s="4" customFormat="1">
       <c r="B215" s="22"/>
       <c r="C215" s="5"/>
       <c r="D215" s="27"/>
@@ -4091,8 +4636,9 @@
       <c r="H215" s="7"/>
       <c r="I215" s="7"/>
       <c r="J215" s="7"/>
-    </row>
-    <row r="216" spans="2:10" s="4" customFormat="1">
+      <c r="K215" s="52"/>
+    </row>
+    <row r="216" spans="2:11" s="4" customFormat="1">
       <c r="B216" s="22"/>
       <c r="C216" s="5"/>
       <c r="D216" s="27"/>
@@ -4102,8 +4648,9 @@
       <c r="H216" s="7"/>
       <c r="I216" s="7"/>
       <c r="J216" s="7"/>
-    </row>
-    <row r="217" spans="2:10" s="4" customFormat="1">
+      <c r="K216" s="52"/>
+    </row>
+    <row r="217" spans="2:11" s="4" customFormat="1">
       <c r="B217" s="22"/>
       <c r="C217" s="5"/>
       <c r="D217" s="27"/>
@@ -4113,8 +4660,9 @@
       <c r="H217" s="7"/>
       <c r="I217" s="7"/>
       <c r="J217" s="7"/>
-    </row>
-    <row r="218" spans="2:10" s="4" customFormat="1">
+      <c r="K217" s="52"/>
+    </row>
+    <row r="218" spans="2:11" s="4" customFormat="1">
       <c r="B218" s="22"/>
       <c r="C218" s="5"/>
       <c r="D218" s="27"/>
@@ -4124,8 +4672,9 @@
       <c r="H218" s="7"/>
       <c r="I218" s="7"/>
       <c r="J218" s="7"/>
-    </row>
-    <row r="219" spans="2:10" s="4" customFormat="1">
+      <c r="K218" s="52"/>
+    </row>
+    <row r="219" spans="2:11" s="4" customFormat="1">
       <c r="B219" s="22"/>
       <c r="C219" s="5"/>
       <c r="D219" s="27"/>
@@ -4135,8 +4684,9 @@
       <c r="H219" s="7"/>
       <c r="I219" s="7"/>
       <c r="J219" s="7"/>
-    </row>
-    <row r="220" spans="2:10" s="4" customFormat="1">
+      <c r="K219" s="52"/>
+    </row>
+    <row r="220" spans="2:11" s="4" customFormat="1">
       <c r="B220" s="22"/>
       <c r="C220" s="5"/>
       <c r="D220" s="27"/>
@@ -4146,8 +4696,9 @@
       <c r="H220" s="7"/>
       <c r="I220" s="7"/>
       <c r="J220" s="7"/>
-    </row>
-    <row r="221" spans="2:10" s="4" customFormat="1">
+      <c r="K220" s="52"/>
+    </row>
+    <row r="221" spans="2:11" s="4" customFormat="1">
       <c r="B221" s="22"/>
       <c r="C221" s="5"/>
       <c r="D221" s="27"/>
@@ -4157,8 +4708,9 @@
       <c r="H221" s="7"/>
       <c r="I221" s="7"/>
       <c r="J221" s="7"/>
-    </row>
-    <row r="222" spans="2:10" s="4" customFormat="1">
+      <c r="K221" s="52"/>
+    </row>
+    <row r="222" spans="2:11" s="4" customFormat="1">
       <c r="B222" s="22"/>
       <c r="C222" s="5"/>
       <c r="D222" s="27"/>
@@ -4168,8 +4720,9 @@
       <c r="H222" s="7"/>
       <c r="I222" s="7"/>
       <c r="J222" s="7"/>
-    </row>
-    <row r="223" spans="2:10" s="4" customFormat="1">
+      <c r="K222" s="52"/>
+    </row>
+    <row r="223" spans="2:11" s="4" customFormat="1">
       <c r="B223" s="22"/>
       <c r="C223" s="5"/>
       <c r="D223" s="27"/>
@@ -4179,8 +4732,9 @@
       <c r="H223" s="7"/>
       <c r="I223" s="7"/>
       <c r="J223" s="7"/>
-    </row>
-    <row r="224" spans="2:10" s="4" customFormat="1">
+      <c r="K223" s="52"/>
+    </row>
+    <row r="224" spans="2:11" s="4" customFormat="1">
       <c r="B224" s="22"/>
       <c r="C224" s="5"/>
       <c r="D224" s="27"/>
@@ -4190,8 +4744,9 @@
       <c r="H224" s="7"/>
       <c r="I224" s="7"/>
       <c r="J224" s="7"/>
-    </row>
-    <row r="225" spans="2:10" s="4" customFormat="1">
+      <c r="K224" s="52"/>
+    </row>
+    <row r="225" spans="2:11" s="4" customFormat="1">
       <c r="B225" s="22"/>
       <c r="C225" s="5"/>
       <c r="D225" s="27"/>
@@ -4201,8 +4756,9 @@
       <c r="H225" s="7"/>
       <c r="I225" s="7"/>
       <c r="J225" s="7"/>
-    </row>
-    <row r="226" spans="2:10" s="4" customFormat="1">
+      <c r="K225" s="52"/>
+    </row>
+    <row r="226" spans="2:11" s="4" customFormat="1">
       <c r="B226" s="22"/>
       <c r="C226" s="5"/>
       <c r="D226" s="27"/>
@@ -4212,8 +4768,9 @@
       <c r="H226" s="7"/>
       <c r="I226" s="7"/>
       <c r="J226" s="7"/>
-    </row>
-    <row r="227" spans="2:10" s="4" customFormat="1">
+      <c r="K226" s="52"/>
+    </row>
+    <row r="227" spans="2:11" s="4" customFormat="1">
       <c r="B227" s="22"/>
       <c r="C227" s="5"/>
       <c r="D227" s="27"/>
@@ -4223,8 +4780,9 @@
       <c r="H227" s="7"/>
       <c r="I227" s="7"/>
       <c r="J227" s="7"/>
-    </row>
-    <row r="228" spans="2:10" s="4" customFormat="1">
+      <c r="K227" s="52"/>
+    </row>
+    <row r="228" spans="2:11" s="4" customFormat="1">
       <c r="B228" s="22"/>
       <c r="C228" s="5"/>
       <c r="D228" s="27"/>
@@ -4234,8 +4792,9 @@
       <c r="H228" s="7"/>
       <c r="I228" s="7"/>
       <c r="J228" s="7"/>
-    </row>
-    <row r="229" spans="2:10" s="4" customFormat="1">
+      <c r="K228" s="52"/>
+    </row>
+    <row r="229" spans="2:11" s="4" customFormat="1">
       <c r="B229" s="22"/>
       <c r="C229" s="5"/>
       <c r="D229" s="27"/>
@@ -4245,8 +4804,9 @@
       <c r="H229" s="7"/>
       <c r="I229" s="7"/>
       <c r="J229" s="7"/>
-    </row>
-    <row r="230" spans="2:10" s="4" customFormat="1">
+      <c r="K229" s="52"/>
+    </row>
+    <row r="230" spans="2:11" s="4" customFormat="1">
       <c r="B230" s="22"/>
       <c r="C230" s="5"/>
       <c r="D230" s="27"/>
@@ -4256,8 +4816,9 @@
       <c r="H230" s="7"/>
       <c r="I230" s="7"/>
       <c r="J230" s="7"/>
-    </row>
-    <row r="231" spans="2:10" s="4" customFormat="1">
+      <c r="K230" s="52"/>
+    </row>
+    <row r="231" spans="2:11" s="4" customFormat="1">
       <c r="B231" s="22"/>
       <c r="C231" s="5"/>
       <c r="D231" s="27"/>
@@ -4267,8 +4828,9 @@
       <c r="H231" s="7"/>
       <c r="I231" s="7"/>
       <c r="J231" s="7"/>
-    </row>
-    <row r="232" spans="2:10" s="4" customFormat="1">
+      <c r="K231" s="52"/>
+    </row>
+    <row r="232" spans="2:11" s="4" customFormat="1">
       <c r="B232" s="22"/>
       <c r="C232" s="5"/>
       <c r="D232" s="27"/>
@@ -4278,8 +4840,9 @@
       <c r="H232" s="7"/>
       <c r="I232" s="7"/>
       <c r="J232" s="7"/>
-    </row>
-    <row r="233" spans="2:10" s="4" customFormat="1">
+      <c r="K232" s="52"/>
+    </row>
+    <row r="233" spans="2:11" s="4" customFormat="1">
       <c r="B233" s="22"/>
       <c r="C233" s="5"/>
       <c r="D233" s="27"/>
@@ -4289,8 +4852,9 @@
       <c r="H233" s="7"/>
       <c r="I233" s="7"/>
       <c r="J233" s="7"/>
-    </row>
-    <row r="234" spans="2:10" s="4" customFormat="1">
+      <c r="K233" s="52"/>
+    </row>
+    <row r="234" spans="2:11" s="4" customFormat="1">
       <c r="B234" s="22"/>
       <c r="C234" s="5"/>
       <c r="D234" s="27"/>
@@ -4300,8 +4864,9 @@
       <c r="H234" s="7"/>
       <c r="I234" s="7"/>
       <c r="J234" s="7"/>
-    </row>
-    <row r="235" spans="2:10" s="4" customFormat="1">
+      <c r="K234" s="52"/>
+    </row>
+    <row r="235" spans="2:11" s="4" customFormat="1">
       <c r="B235" s="22"/>
       <c r="C235" s="5"/>
       <c r="D235" s="27"/>
@@ -4311,8 +4876,9 @@
       <c r="H235" s="7"/>
       <c r="I235" s="7"/>
       <c r="J235" s="7"/>
-    </row>
-    <row r="236" spans="2:10" s="4" customFormat="1">
+      <c r="K235" s="52"/>
+    </row>
+    <row r="236" spans="2:11" s="4" customFormat="1">
       <c r="B236" s="22"/>
       <c r="C236" s="5"/>
       <c r="D236" s="27"/>
@@ -4322,8 +4888,9 @@
       <c r="H236" s="7"/>
       <c r="I236" s="7"/>
       <c r="J236" s="7"/>
-    </row>
-    <row r="237" spans="2:10" s="4" customFormat="1">
+      <c r="K236" s="52"/>
+    </row>
+    <row r="237" spans="2:11" s="4" customFormat="1">
       <c r="B237" s="22"/>
       <c r="C237" s="5"/>
       <c r="D237" s="27"/>
@@ -4333,8 +4900,9 @@
       <c r="H237" s="7"/>
       <c r="I237" s="7"/>
       <c r="J237" s="7"/>
-    </row>
-    <row r="238" spans="2:10" s="4" customFormat="1">
+      <c r="K237" s="52"/>
+    </row>
+    <row r="238" spans="2:11" s="4" customFormat="1">
       <c r="B238" s="22"/>
       <c r="C238" s="5"/>
       <c r="D238" s="27"/>
@@ -4344,8 +4912,9 @@
       <c r="H238" s="7"/>
       <c r="I238" s="7"/>
       <c r="J238" s="7"/>
-    </row>
-    <row r="239" spans="2:10" s="4" customFormat="1">
+      <c r="K238" s="52"/>
+    </row>
+    <row r="239" spans="2:11" s="4" customFormat="1">
       <c r="B239" s="22"/>
       <c r="C239" s="5"/>
       <c r="D239" s="27"/>
@@ -4355,8 +4924,9 @@
       <c r="H239" s="7"/>
       <c r="I239" s="7"/>
       <c r="J239" s="7"/>
-    </row>
-    <row r="240" spans="2:10" s="4" customFormat="1">
+      <c r="K239" s="52"/>
+    </row>
+    <row r="240" spans="2:11" s="4" customFormat="1">
       <c r="B240" s="22"/>
       <c r="C240" s="5"/>
       <c r="D240" s="27"/>
@@ -4366,8 +4936,9 @@
       <c r="H240" s="7"/>
       <c r="I240" s="7"/>
       <c r="J240" s="7"/>
-    </row>
-    <row r="241" spans="2:10" s="4" customFormat="1">
+      <c r="K240" s="52"/>
+    </row>
+    <row r="241" spans="2:11" s="4" customFormat="1">
       <c r="B241" s="22"/>
       <c r="C241" s="5"/>
       <c r="D241" s="27"/>
@@ -4377,8 +4948,9 @@
       <c r="H241" s="7"/>
       <c r="I241" s="7"/>
       <c r="J241" s="7"/>
-    </row>
-    <row r="242" spans="2:10" s="4" customFormat="1">
+      <c r="K241" s="52"/>
+    </row>
+    <row r="242" spans="2:11" s="4" customFormat="1">
       <c r="B242" s="22"/>
       <c r="C242" s="5"/>
       <c r="D242" s="27"/>
@@ -4388,8 +4960,9 @@
       <c r="H242" s="7"/>
       <c r="I242" s="7"/>
       <c r="J242" s="7"/>
-    </row>
-    <row r="243" spans="2:10" s="4" customFormat="1">
+      <c r="K242" s="52"/>
+    </row>
+    <row r="243" spans="2:11" s="4" customFormat="1">
       <c r="B243" s="22"/>
       <c r="C243" s="5"/>
       <c r="D243" s="27"/>
@@ -4399,8 +4972,9 @@
       <c r="H243" s="7"/>
       <c r="I243" s="7"/>
       <c r="J243" s="7"/>
-    </row>
-    <row r="244" spans="2:10" s="4" customFormat="1">
+      <c r="K243" s="52"/>
+    </row>
+    <row r="244" spans="2:11" s="4" customFormat="1">
       <c r="B244" s="22"/>
       <c r="C244" s="5"/>
       <c r="D244" s="27"/>
@@ -4410,8 +4984,9 @@
       <c r="H244" s="7"/>
       <c r="I244" s="7"/>
       <c r="J244" s="7"/>
-    </row>
-    <row r="245" spans="2:10" s="4" customFormat="1">
+      <c r="K244" s="52"/>
+    </row>
+    <row r="245" spans="2:11" s="4" customFormat="1">
       <c r="B245" s="22"/>
       <c r="C245" s="5"/>
       <c r="D245" s="27"/>
@@ -4421,8 +4996,9 @@
       <c r="H245" s="7"/>
       <c r="I245" s="7"/>
       <c r="J245" s="7"/>
-    </row>
-    <row r="246" spans="2:10" s="4" customFormat="1">
+      <c r="K245" s="52"/>
+    </row>
+    <row r="246" spans="2:11" s="4" customFormat="1">
       <c r="B246" s="22"/>
       <c r="C246" s="5"/>
       <c r="D246" s="27"/>
@@ -4432,8 +5008,9 @@
       <c r="H246" s="7"/>
       <c r="I246" s="7"/>
       <c r="J246" s="7"/>
-    </row>
-    <row r="247" spans="2:10" s="4" customFormat="1">
+      <c r="K246" s="52"/>
+    </row>
+    <row r="247" spans="2:11" s="4" customFormat="1">
       <c r="B247" s="22"/>
       <c r="C247" s="5"/>
       <c r="D247" s="27"/>
@@ -4443,8 +5020,9 @@
       <c r="H247" s="7"/>
       <c r="I247" s="7"/>
       <c r="J247" s="7"/>
-    </row>
-    <row r="248" spans="2:10" s="4" customFormat="1">
+      <c r="K247" s="52"/>
+    </row>
+    <row r="248" spans="2:11" s="4" customFormat="1">
       <c r="B248" s="22"/>
       <c r="C248" s="5"/>
       <c r="D248" s="27"/>
@@ -4454,8 +5032,9 @@
       <c r="H248" s="7"/>
       <c r="I248" s="7"/>
       <c r="J248" s="7"/>
-    </row>
-    <row r="249" spans="2:10" s="4" customFormat="1">
+      <c r="K248" s="52"/>
+    </row>
+    <row r="249" spans="2:11" s="4" customFormat="1">
       <c r="B249" s="22"/>
       <c r="C249" s="5"/>
       <c r="D249" s="27"/>
@@ -4465,8 +5044,9 @@
       <c r="H249" s="7"/>
       <c r="I249" s="7"/>
       <c r="J249" s="7"/>
-    </row>
-    <row r="250" spans="2:10" s="4" customFormat="1">
+      <c r="K249" s="52"/>
+    </row>
+    <row r="250" spans="2:11" s="4" customFormat="1">
       <c r="B250" s="22"/>
       <c r="C250" s="5"/>
       <c r="D250" s="27"/>
@@ -4476,8 +5056,9 @@
       <c r="H250" s="7"/>
       <c r="I250" s="7"/>
       <c r="J250" s="7"/>
-    </row>
-    <row r="251" spans="2:10" s="4" customFormat="1">
+      <c r="K250" s="52"/>
+    </row>
+    <row r="251" spans="2:11" s="4" customFormat="1">
       <c r="B251" s="22"/>
       <c r="C251" s="5"/>
       <c r="D251" s="27"/>
@@ -4487,8 +5068,9 @@
       <c r="H251" s="7"/>
       <c r="I251" s="7"/>
       <c r="J251" s="7"/>
-    </row>
-    <row r="252" spans="2:10" s="4" customFormat="1">
+      <c r="K251" s="52"/>
+    </row>
+    <row r="252" spans="2:11" s="4" customFormat="1">
       <c r="B252" s="22"/>
       <c r="C252" s="5"/>
       <c r="D252" s="27"/>
@@ -4498,8 +5080,9 @@
       <c r="H252" s="7"/>
       <c r="I252" s="7"/>
       <c r="J252" s="7"/>
-    </row>
-    <row r="253" spans="2:10" s="4" customFormat="1">
+      <c r="K252" s="52"/>
+    </row>
+    <row r="253" spans="2:11" s="4" customFormat="1">
       <c r="B253" s="22"/>
       <c r="C253" s="5"/>
       <c r="D253" s="27"/>
@@ -4509,8 +5092,9 @@
       <c r="H253" s="7"/>
       <c r="I253" s="7"/>
       <c r="J253" s="7"/>
-    </row>
-    <row r="254" spans="2:10" s="4" customFormat="1">
+      <c r="K253" s="52"/>
+    </row>
+    <row r="254" spans="2:11" s="4" customFormat="1">
       <c r="B254" s="22"/>
       <c r="C254" s="5"/>
       <c r="D254" s="27"/>
@@ -4520,8 +5104,9 @@
       <c r="H254" s="7"/>
       <c r="I254" s="7"/>
       <c r="J254" s="7"/>
-    </row>
-    <row r="255" spans="2:10" s="4" customFormat="1">
+      <c r="K254" s="52"/>
+    </row>
+    <row r="255" spans="2:11" s="4" customFormat="1">
       <c r="B255" s="22"/>
       <c r="C255" s="5"/>
       <c r="D255" s="27"/>
@@ -4531,8 +5116,9 @@
       <c r="H255" s="7"/>
       <c r="I255" s="7"/>
       <c r="J255" s="7"/>
-    </row>
-    <row r="256" spans="2:10" s="4" customFormat="1">
+      <c r="K255" s="52"/>
+    </row>
+    <row r="256" spans="2:11" s="4" customFormat="1">
       <c r="B256" s="22"/>
       <c r="C256" s="5"/>
       <c r="D256" s="27"/>
@@ -4542,8 +5128,9 @@
       <c r="H256" s="7"/>
       <c r="I256" s="7"/>
       <c r="J256" s="7"/>
-    </row>
-    <row r="257" spans="2:10" s="4" customFormat="1">
+      <c r="K256" s="52"/>
+    </row>
+    <row r="257" spans="2:11" s="4" customFormat="1">
       <c r="B257" s="22"/>
       <c r="C257" s="5"/>
       <c r="D257" s="27"/>
@@ -4553,8 +5140,9 @@
       <c r="H257" s="7"/>
       <c r="I257" s="7"/>
       <c r="J257" s="7"/>
-    </row>
-    <row r="258" spans="2:10" s="4" customFormat="1">
+      <c r="K257" s="52"/>
+    </row>
+    <row r="258" spans="2:11" s="4" customFormat="1">
       <c r="B258" s="22"/>
       <c r="C258" s="5"/>
       <c r="D258" s="27"/>
@@ -4564,8 +5152,9 @@
       <c r="H258" s="7"/>
       <c r="I258" s="7"/>
       <c r="J258" s="7"/>
-    </row>
-    <row r="259" spans="2:10" s="4" customFormat="1">
+      <c r="K258" s="52"/>
+    </row>
+    <row r="259" spans="2:11" s="4" customFormat="1">
       <c r="B259" s="22"/>
       <c r="C259" s="5"/>
       <c r="D259" s="27"/>
@@ -4575,8 +5164,9 @@
       <c r="H259" s="7"/>
       <c r="I259" s="7"/>
       <c r="J259" s="7"/>
-    </row>
-    <row r="260" spans="2:10" s="4" customFormat="1">
+      <c r="K259" s="52"/>
+    </row>
+    <row r="260" spans="2:11" s="4" customFormat="1">
       <c r="B260" s="22"/>
       <c r="C260" s="5"/>
       <c r="D260" s="27"/>
@@ -4586,8 +5176,9 @@
       <c r="H260" s="7"/>
       <c r="I260" s="7"/>
       <c r="J260" s="7"/>
-    </row>
-    <row r="261" spans="2:10" s="4" customFormat="1">
+      <c r="K260" s="52"/>
+    </row>
+    <row r="261" spans="2:11" s="4" customFormat="1">
       <c r="B261" s="22"/>
       <c r="C261" s="5"/>
       <c r="D261" s="27"/>
@@ -4597,8 +5188,9 @@
       <c r="H261" s="7"/>
       <c r="I261" s="7"/>
       <c r="J261" s="7"/>
-    </row>
-    <row r="262" spans="2:10" s="4" customFormat="1">
+      <c r="K261" s="52"/>
+    </row>
+    <row r="262" spans="2:11" s="4" customFormat="1">
       <c r="B262" s="22"/>
       <c r="C262" s="5"/>
       <c r="D262" s="27"/>
@@ -4608,8 +5200,9 @@
       <c r="H262" s="7"/>
       <c r="I262" s="7"/>
       <c r="J262" s="7"/>
-    </row>
-    <row r="263" spans="2:10" s="4" customFormat="1">
+      <c r="K262" s="52"/>
+    </row>
+    <row r="263" spans="2:11" s="4" customFormat="1">
       <c r="B263" s="22"/>
       <c r="C263" s="5"/>
       <c r="D263" s="27"/>
@@ -4619,8 +5212,9 @@
       <c r="H263" s="7"/>
       <c r="I263" s="7"/>
       <c r="J263" s="7"/>
-    </row>
-    <row r="264" spans="2:10" s="4" customFormat="1">
+      <c r="K263" s="52"/>
+    </row>
+    <row r="264" spans="2:11" s="4" customFormat="1">
       <c r="B264" s="22"/>
       <c r="C264" s="5"/>
       <c r="D264" s="27"/>
@@ -4630,8 +5224,9 @@
       <c r="H264" s="7"/>
       <c r="I264" s="7"/>
       <c r="J264" s="7"/>
-    </row>
-    <row r="265" spans="2:10" s="4" customFormat="1">
+      <c r="K264" s="52"/>
+    </row>
+    <row r="265" spans="2:11" s="4" customFormat="1">
       <c r="B265" s="22"/>
       <c r="C265" s="5"/>
       <c r="D265" s="27"/>
@@ -4641,8 +5236,9 @@
       <c r="H265" s="7"/>
       <c r="I265" s="7"/>
       <c r="J265" s="7"/>
-    </row>
-    <row r="266" spans="2:10" s="4" customFormat="1">
+      <c r="K265" s="52"/>
+    </row>
+    <row r="266" spans="2:11" s="4" customFormat="1">
       <c r="B266" s="22"/>
       <c r="C266" s="5"/>
       <c r="D266" s="27"/>
@@ -4652,8 +5248,9 @@
       <c r="H266" s="7"/>
       <c r="I266" s="7"/>
       <c r="J266" s="7"/>
-    </row>
-    <row r="267" spans="2:10" s="4" customFormat="1">
+      <c r="K266" s="52"/>
+    </row>
+    <row r="267" spans="2:11" s="4" customFormat="1">
       <c r="B267" s="22"/>
       <c r="C267" s="5"/>
       <c r="D267" s="27"/>
@@ -4663,8 +5260,9 @@
       <c r="H267" s="7"/>
       <c r="I267" s="7"/>
       <c r="J267" s="7"/>
-    </row>
-    <row r="268" spans="2:10" s="4" customFormat="1">
+      <c r="K267" s="52"/>
+    </row>
+    <row r="268" spans="2:11" s="4" customFormat="1">
       <c r="B268" s="22"/>
       <c r="C268" s="5"/>
       <c r="D268" s="27"/>
@@ -4674,8 +5272,9 @@
       <c r="H268" s="7"/>
       <c r="I268" s="7"/>
       <c r="J268" s="7"/>
-    </row>
-    <row r="269" spans="2:10" s="4" customFormat="1">
+      <c r="K268" s="52"/>
+    </row>
+    <row r="269" spans="2:11" s="4" customFormat="1">
       <c r="B269" s="22"/>
       <c r="C269" s="5"/>
       <c r="D269" s="27"/>
@@ -4685,8 +5284,9 @@
       <c r="H269" s="7"/>
       <c r="I269" s="7"/>
       <c r="J269" s="7"/>
-    </row>
-    <row r="270" spans="2:10" s="4" customFormat="1">
+      <c r="K269" s="52"/>
+    </row>
+    <row r="270" spans="2:11" s="4" customFormat="1">
       <c r="B270" s="22"/>
       <c r="C270" s="5"/>
       <c r="D270" s="27"/>
@@ -4696,8 +5296,9 @@
       <c r="H270" s="7"/>
       <c r="I270" s="7"/>
       <c r="J270" s="7"/>
-    </row>
-    <row r="271" spans="2:10" s="4" customFormat="1">
+      <c r="K270" s="52"/>
+    </row>
+    <row r="271" spans="2:11" s="4" customFormat="1">
       <c r="B271" s="22"/>
       <c r="C271" s="5"/>
       <c r="D271" s="27"/>
@@ -4707,8 +5308,9 @@
       <c r="H271" s="7"/>
       <c r="I271" s="7"/>
       <c r="J271" s="7"/>
-    </row>
-    <row r="272" spans="2:10" s="4" customFormat="1">
+      <c r="K271" s="52"/>
+    </row>
+    <row r="272" spans="2:11" s="4" customFormat="1">
       <c r="B272" s="22"/>
       <c r="C272" s="5"/>
       <c r="D272" s="27"/>
@@ -4718,6 +5320,7 @@
       <c r="H272" s="7"/>
       <c r="I272" s="7"/>
       <c r="J272" s="7"/>
+      <c r="K272" s="52"/>
     </row>
     <row r="273" spans="2:240" s="4" customFormat="1">
       <c r="B273" s="22"/>
@@ -4729,6 +5332,7 @@
       <c r="H273" s="7"/>
       <c r="I273" s="7"/>
       <c r="J273" s="7"/>
+      <c r="K273" s="52"/>
     </row>
     <row r="274" spans="2:240" s="4" customFormat="1">
       <c r="B274" s="22"/>
@@ -4740,6 +5344,7 @@
       <c r="H274" s="7"/>
       <c r="I274" s="7"/>
       <c r="J274" s="7"/>
+      <c r="K274" s="52"/>
     </row>
     <row r="275" spans="2:240" s="4" customFormat="1">
       <c r="B275" s="22"/>
@@ -4751,6 +5356,7 @@
       <c r="H275" s="7"/>
       <c r="I275" s="7"/>
       <c r="J275" s="7"/>
+      <c r="K275" s="52"/>
     </row>
     <row r="276" spans="2:240" s="4" customFormat="1">
       <c r="B276" s="22"/>
@@ -4762,6 +5368,7 @@
       <c r="H276" s="7"/>
       <c r="I276" s="7"/>
       <c r="J276" s="7"/>
+      <c r="K276" s="52"/>
     </row>
     <row r="277" spans="2:240" s="4" customFormat="1">
       <c r="B277" s="22"/>
@@ -4773,6 +5380,7 @@
       <c r="H277" s="7"/>
       <c r="I277" s="7"/>
       <c r="J277" s="7"/>
+      <c r="K277" s="52"/>
     </row>
     <row r="278" spans="2:240" s="4" customFormat="1">
       <c r="B278" s="22"/>
@@ -4784,6 +5392,7 @@
       <c r="H278" s="7"/>
       <c r="I278" s="7"/>
       <c r="J278" s="7"/>
+      <c r="K278" s="52"/>
     </row>
     <row r="279" spans="2:240" s="4" customFormat="1">
       <c r="B279" s="22"/>
@@ -4795,6 +5404,7 @@
       <c r="H279" s="7"/>
       <c r="I279" s="7"/>
       <c r="J279" s="7"/>
+      <c r="K279" s="52"/>
     </row>
     <row r="280" spans="2:240" s="4" customFormat="1">
       <c r="B280" s="22"/>
@@ -4806,17 +5416,17 @@
       <c r="H280" s="7"/>
       <c r="I280" s="7"/>
       <c r="J280" s="7"/>
-    </row>
-    <row r="281" spans="2:240" s="4" customFormat="1">
-      <c r="B281" s="22"/>
-      <c r="C281" s="5"/>
-      <c r="D281" s="27"/>
-      <c r="E281" s="6"/>
-      <c r="F281" s="6"/>
-      <c r="G281" s="7"/>
-      <c r="H281" s="7"/>
-      <c r="I281" s="7"/>
-      <c r="J281" s="7"/>
+      <c r="K280" s="52"/>
+    </row>
+    <row r="281" spans="2:240">
+      <c r="HY281" s="4"/>
+      <c r="HZ281" s="4"/>
+      <c r="IA281" s="4"/>
+      <c r="IB281" s="4"/>
+      <c r="IC281" s="4"/>
+      <c r="ID281" s="4"/>
+      <c r="IE281" s="4"/>
+      <c r="IF281" s="4"/>
     </row>
     <row r="282" spans="2:240">
       <c r="HY282" s="4"/>
@@ -8658,18 +9268,8 @@
       <c r="IE665" s="4"/>
       <c r="IF665" s="4"/>
     </row>
-    <row r="666" spans="233:240">
-      <c r="HY666" s="4"/>
-      <c r="HZ666" s="4"/>
-      <c r="IA666" s="4"/>
-      <c r="IB666" s="4"/>
-      <c r="IC666" s="4"/>
-      <c r="ID666" s="4"/>
-      <c r="IE666" s="4"/>
-      <c r="IF666" s="4"/>
-    </row>
-    <row r="65362" spans="9:9">
-      <c r="I65362" s="11" t="s">
+    <row r="65361" spans="9:9">
+      <c r="I65361" s="11" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>